<commit_message>
Release candidate for 1.4.0.0
Release candidate for 1.4.0.0 with autotracker
</commit_message>
<xml_diff>
--- a/autotracking/Switches.xlsx
+++ b/autotracking/Switches.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21727"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Apokalysme\LaunchMyCraft\git_repository\iogr_emotracker_apokalysme\autotracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0367EF9D-037F-42D2-A2B3-DCB3E7381B0A}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E84D46-FE15-4F9E-AB77-9E7E47873E45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="315" windowWidth="15060" windowHeight="14655" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Switches_New" sheetId="4" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1830" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="720">
   <si>
     <t>ID</t>
   </si>
@@ -2201,6 +2201,9 @@
   </si>
   <si>
     <t>0x7E0A41</t>
+  </si>
+  <si>
+    <t>Talking to Teacher</t>
   </si>
 </sst>
 </file>
@@ -3673,49 +3676,19 @@
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
@@ -3724,13 +3697,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
@@ -3748,16 +3721,28 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3778,20 +3763,38 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -3806,6 +3809,9 @@
     </dxf>
     <dxf>
       <alignment horizontal="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3828,9 +3834,6 @@
         <scheme val="minor"/>
       </font>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -3892,10 +3895,10 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2145C2C-28E7-4729-95B3-33F4F107767B}" name="Tableau3" displayName="Tableau3" ref="B2:H107" totalsRowShown="0" headerRowDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{D2145C2C-28E7-4729-95B3-33F4F107767B}" name="Tableau3" displayName="Tableau3" ref="B2:H107" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B2:H107" xr:uid="{43C0CF75-B856-4CC6-A6A8-EEAC4E75867E}"/>
   <tableColumns count="7">
-    <tableColumn id="1" xr3:uid="{4ED943CA-2B52-4FC9-AC61-1CD9FB02091D}" name="ID" dataDxfId="4"/>
+    <tableColumn id="1" xr3:uid="{4ED943CA-2B52-4FC9-AC61-1CD9FB02091D}" name="ID" dataDxfId="3"/>
     <tableColumn id="2" xr3:uid="{91401FD4-6D61-468F-9530-BF0307C82E28}" name="Place"/>
     <tableColumn id="3" xr3:uid="{20A3E718-7616-4DC8-817B-C099CB3B8912}" name="Zone"/>
     <tableColumn id="4" xr3:uid="{96C9C31E-3EEE-4C51-80E9-F6B671DAD769}" name="Spot"/>
@@ -4233,9 +4236,9 @@
   </sheetPr>
   <dimension ref="A1:P1237"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I32" sqref="H32:I32"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -4309,16 +4312,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="203" t="s">
+      <c r="D2" s="188" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="200"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="189"/>
+      <c r="K2" s="190"/>
       <c r="M2" s="81" t="s">
         <v>7</v>
       </c>
@@ -4336,14 +4339,14 @@
         <f t="shared" ref="C3:C33" si="1">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="204"/>
-      <c r="E3" s="205"/>
-      <c r="F3" s="205"/>
-      <c r="G3" s="205"/>
-      <c r="H3" s="205"/>
-      <c r="I3" s="205"/>
-      <c r="J3" s="205"/>
-      <c r="K3" s="206"/>
+      <c r="D3" s="194"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="I3" s="195"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="196"/>
       <c r="M3" s="81" t="s">
         <v>8</v>
       </c>
@@ -4585,7 +4588,9 @@
         <v>50</v>
       </c>
       <c r="J9" s="162"/>
-      <c r="K9" s="162"/>
+      <c r="K9" s="166" t="s">
+        <v>719</v>
+      </c>
       <c r="M9" s="6">
         <v>38</v>
       </c>
@@ -10400,16 +10405,16 @@
         <v>AA6</v>
       </c>
       <c r="C168" s="13"/>
-      <c r="D168" s="184" t="s">
+      <c r="D168" s="221" t="s">
         <v>348</v>
       </c>
-      <c r="E168" s="184"/>
-      <c r="F168" s="184"/>
-      <c r="G168" s="184"/>
-      <c r="H168" s="184"/>
-      <c r="I168" s="184"/>
-      <c r="J168" s="184"/>
-      <c r="K168" s="184"/>
+      <c r="E168" s="221"/>
+      <c r="F168" s="221"/>
+      <c r="G168" s="221"/>
+      <c r="H168" s="221"/>
+      <c r="I168" s="221"/>
+      <c r="J168" s="221"/>
+      <c r="K168" s="221"/>
     </row>
     <row r="169" spans="1:15">
       <c r="A169" s="12">
@@ -10535,16 +10540,16 @@
         <v>AAD</v>
       </c>
       <c r="C175" s="13"/>
-      <c r="D175" s="184" t="s">
+      <c r="D175" s="221" t="s">
         <v>349</v>
       </c>
-      <c r="E175" s="184"/>
-      <c r="F175" s="184"/>
-      <c r="G175" s="184"/>
-      <c r="H175" s="184"/>
-      <c r="I175" s="184"/>
-      <c r="J175" s="184"/>
-      <c r="K175" s="184"/>
+      <c r="E175" s="221"/>
+      <c r="F175" s="221"/>
+      <c r="G175" s="221"/>
+      <c r="H175" s="221"/>
+      <c r="I175" s="221"/>
+      <c r="J175" s="221"/>
+      <c r="K175" s="221"/>
     </row>
     <row r="176" spans="1:15">
       <c r="A176" s="12">
@@ -10597,16 +10602,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="38"/>
-      <c r="D178" s="185" t="s">
+      <c r="D178" s="222" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="184"/>
-      <c r="F178" s="184"/>
-      <c r="G178" s="184"/>
-      <c r="H178" s="184"/>
-      <c r="I178" s="184"/>
-      <c r="J178" s="184"/>
-      <c r="K178" s="184"/>
+      <c r="E178" s="221"/>
+      <c r="F178" s="221"/>
+      <c r="G178" s="221"/>
+      <c r="H178" s="221"/>
+      <c r="I178" s="221"/>
+      <c r="J178" s="221"/>
+      <c r="K178" s="221"/>
       <c r="L178" t="s">
         <v>424</v>
       </c>
@@ -10678,16 +10683,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="186" t="s">
+      <c r="D182" s="204" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="187"/>
-      <c r="F182" s="187"/>
-      <c r="G182" s="187"/>
-      <c r="H182" s="187"/>
-      <c r="I182" s="187"/>
-      <c r="J182" s="187"/>
-      <c r="K182" s="188"/>
+      <c r="E182" s="205"/>
+      <c r="F182" s="205"/>
+      <c r="G182" s="205"/>
+      <c r="H182" s="205"/>
+      <c r="I182" s="205"/>
+      <c r="J182" s="205"/>
+      <c r="K182" s="206"/>
     </row>
     <row r="183" spans="1:15">
       <c r="A183" s="12">
@@ -10699,16 +10704,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="186" t="s">
+      <c r="D183" s="204" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="187"/>
-      <c r="F183" s="187"/>
-      <c r="G183" s="187"/>
-      <c r="H183" s="187"/>
-      <c r="I183" s="187"/>
-      <c r="J183" s="187"/>
-      <c r="K183" s="188"/>
+      <c r="E183" s="205"/>
+      <c r="F183" s="205"/>
+      <c r="G183" s="205"/>
+      <c r="H183" s="205"/>
+      <c r="I183" s="205"/>
+      <c r="J183" s="205"/>
+      <c r="K183" s="206"/>
     </row>
     <row r="184" spans="1:15">
       <c r="A184" s="12">
@@ -10720,16 +10725,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="186" t="s">
+      <c r="D184" s="204" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="187"/>
-      <c r="F184" s="187"/>
-      <c r="G184" s="187"/>
-      <c r="H184" s="187"/>
-      <c r="I184" s="187"/>
-      <c r="J184" s="187"/>
-      <c r="K184" s="188"/>
+      <c r="E184" s="205"/>
+      <c r="F184" s="205"/>
+      <c r="G184" s="205"/>
+      <c r="H184" s="205"/>
+      <c r="I184" s="205"/>
+      <c r="J184" s="205"/>
+      <c r="K184" s="206"/>
     </row>
     <row r="185" spans="1:15">
       <c r="A185" s="12">
@@ -10741,16 +10746,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="186" t="s">
+      <c r="D185" s="204" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="187"/>
-      <c r="F185" s="187"/>
-      <c r="G185" s="187"/>
-      <c r="H185" s="187"/>
-      <c r="I185" s="187"/>
-      <c r="J185" s="187"/>
-      <c r="K185" s="188"/>
+      <c r="E185" s="205"/>
+      <c r="F185" s="205"/>
+      <c r="G185" s="205"/>
+      <c r="H185" s="205"/>
+      <c r="I185" s="205"/>
+      <c r="J185" s="205"/>
+      <c r="K185" s="206"/>
     </row>
     <row r="186" spans="1:15">
       <c r="A186" s="12">
@@ -10762,16 +10767,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="186" t="s">
+      <c r="D186" s="204" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="187"/>
-      <c r="F186" s="187"/>
-      <c r="G186" s="187"/>
-      <c r="H186" s="187"/>
-      <c r="I186" s="187"/>
-      <c r="J186" s="187"/>
-      <c r="K186" s="188"/>
+      <c r="E186" s="205"/>
+      <c r="F186" s="205"/>
+      <c r="G186" s="205"/>
+      <c r="H186" s="205"/>
+      <c r="I186" s="205"/>
+      <c r="J186" s="205"/>
+      <c r="K186" s="206"/>
     </row>
     <row r="187" spans="1:15">
       <c r="A187" s="12">
@@ -10783,16 +10788,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="186" t="s">
+      <c r="D187" s="204" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="187"/>
-      <c r="F187" s="187"/>
-      <c r="G187" s="187"/>
-      <c r="H187" s="187"/>
-      <c r="I187" s="187"/>
-      <c r="J187" s="187"/>
-      <c r="K187" s="188"/>
+      <c r="E187" s="205"/>
+      <c r="F187" s="205"/>
+      <c r="G187" s="205"/>
+      <c r="H187" s="205"/>
+      <c r="I187" s="205"/>
+      <c r="J187" s="205"/>
+      <c r="K187" s="206"/>
     </row>
     <row r="188" spans="1:15">
       <c r="A188" s="12">
@@ -10804,16 +10809,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="186" t="s">
+      <c r="D188" s="204" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="187"/>
-      <c r="F188" s="187"/>
-      <c r="G188" s="187"/>
-      <c r="H188" s="187"/>
-      <c r="I188" s="187"/>
-      <c r="J188" s="187"/>
-      <c r="K188" s="188"/>
+      <c r="E188" s="205"/>
+      <c r="F188" s="205"/>
+      <c r="G188" s="205"/>
+      <c r="H188" s="205"/>
+      <c r="I188" s="205"/>
+      <c r="J188" s="205"/>
+      <c r="K188" s="206"/>
     </row>
     <row r="189" spans="1:15">
       <c r="A189" s="12">
@@ -10825,16 +10830,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="186" t="s">
+      <c r="D189" s="204" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="187"/>
-      <c r="F189" s="187"/>
-      <c r="G189" s="187"/>
-      <c r="H189" s="187"/>
-      <c r="I189" s="187"/>
-      <c r="J189" s="187"/>
-      <c r="K189" s="188"/>
+      <c r="E189" s="205"/>
+      <c r="F189" s="205"/>
+      <c r="G189" s="205"/>
+      <c r="H189" s="205"/>
+      <c r="I189" s="205"/>
+      <c r="J189" s="205"/>
+      <c r="K189" s="206"/>
     </row>
     <row r="190" spans="1:15">
       <c r="A190" s="12">
@@ -10846,16 +10851,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="186" t="s">
+      <c r="D190" s="204" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="187"/>
-      <c r="F190" s="187"/>
-      <c r="G190" s="187"/>
-      <c r="H190" s="187"/>
-      <c r="I190" s="187"/>
-      <c r="J190" s="187"/>
-      <c r="K190" s="188"/>
+      <c r="E190" s="205"/>
+      <c r="F190" s="205"/>
+      <c r="G190" s="205"/>
+      <c r="H190" s="205"/>
+      <c r="I190" s="205"/>
+      <c r="J190" s="205"/>
+      <c r="K190" s="206"/>
     </row>
     <row r="191" spans="1:15">
       <c r="A191" s="12">
@@ -10867,16 +10872,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="186" t="s">
+      <c r="D191" s="204" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="187"/>
-      <c r="F191" s="187"/>
-      <c r="G191" s="187"/>
-      <c r="H191" s="187"/>
-      <c r="I191" s="187"/>
-      <c r="J191" s="187"/>
-      <c r="K191" s="188"/>
+      <c r="E191" s="205"/>
+      <c r="F191" s="205"/>
+      <c r="G191" s="205"/>
+      <c r="H191" s="205"/>
+      <c r="I191" s="205"/>
+      <c r="J191" s="205"/>
+      <c r="K191" s="206"/>
     </row>
     <row r="192" spans="1:15">
       <c r="A192" s="12">
@@ -10888,16 +10893,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="186" t="s">
+      <c r="D192" s="204" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="187"/>
-      <c r="F192" s="187"/>
-      <c r="G192" s="187"/>
-      <c r="H192" s="187"/>
-      <c r="I192" s="187"/>
-      <c r="J192" s="187"/>
-      <c r="K192" s="188"/>
+      <c r="E192" s="205"/>
+      <c r="F192" s="205"/>
+      <c r="G192" s="205"/>
+      <c r="H192" s="205"/>
+      <c r="I192" s="205"/>
+      <c r="J192" s="205"/>
+      <c r="K192" s="206"/>
     </row>
     <row r="193" spans="1:15" s="1" customFormat="1">
       <c r="A193" s="31">
@@ -10909,16 +10914,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="32"/>
-      <c r="D193" s="189" t="s">
+      <c r="D193" s="218" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="190"/>
-      <c r="F193" s="190"/>
-      <c r="G193" s="190"/>
-      <c r="H193" s="190"/>
-      <c r="I193" s="190"/>
-      <c r="J193" s="190"/>
-      <c r="K193" s="191"/>
+      <c r="E193" s="219"/>
+      <c r="F193" s="219"/>
+      <c r="G193" s="219"/>
+      <c r="H193" s="219"/>
+      <c r="I193" s="219"/>
+      <c r="J193" s="219"/>
+      <c r="K193" s="220"/>
       <c r="M193" s="56"/>
       <c r="N193" s="57"/>
       <c r="O193" s="57"/>
@@ -10933,16 +10938,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="38"/>
-      <c r="D194" s="192" t="s">
+      <c r="D194" s="199" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="193"/>
-      <c r="F194" s="193"/>
-      <c r="G194" s="193"/>
-      <c r="H194" s="193"/>
-      <c r="I194" s="193"/>
-      <c r="J194" s="193"/>
-      <c r="K194" s="194"/>
+      <c r="E194" s="192"/>
+      <c r="F194" s="192"/>
+      <c r="G194" s="192"/>
+      <c r="H194" s="192"/>
+      <c r="I194" s="192"/>
+      <c r="J194" s="192"/>
+      <c r="K194" s="200"/>
     </row>
     <row r="195" spans="1:15">
       <c r="A195" s="12">
@@ -10954,16 +10959,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="186" t="s">
+      <c r="D195" s="204" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="187"/>
-      <c r="F195" s="187"/>
-      <c r="G195" s="187"/>
-      <c r="H195" s="187"/>
-      <c r="I195" s="187"/>
-      <c r="J195" s="187"/>
-      <c r="K195" s="188"/>
+      <c r="E195" s="205"/>
+      <c r="F195" s="205"/>
+      <c r="G195" s="205"/>
+      <c r="H195" s="205"/>
+      <c r="I195" s="205"/>
+      <c r="J195" s="205"/>
+      <c r="K195" s="206"/>
     </row>
     <row r="196" spans="1:15">
       <c r="A196" s="12">
@@ -10975,16 +10980,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="186" t="s">
+      <c r="D196" s="204" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="187"/>
-      <c r="F196" s="187"/>
-      <c r="G196" s="187"/>
-      <c r="H196" s="187"/>
-      <c r="I196" s="187"/>
-      <c r="J196" s="187"/>
-      <c r="K196" s="188"/>
+      <c r="E196" s="205"/>
+      <c r="F196" s="205"/>
+      <c r="G196" s="205"/>
+      <c r="H196" s="205"/>
+      <c r="I196" s="205"/>
+      <c r="J196" s="205"/>
+      <c r="K196" s="206"/>
     </row>
     <row r="197" spans="1:15">
       <c r="A197" s="12">
@@ -10996,16 +11001,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="186" t="s">
+      <c r="D197" s="204" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="187"/>
-      <c r="F197" s="187"/>
-      <c r="G197" s="187"/>
-      <c r="H197" s="187"/>
-      <c r="I197" s="187"/>
-      <c r="J197" s="187"/>
-      <c r="K197" s="188"/>
+      <c r="E197" s="205"/>
+      <c r="F197" s="205"/>
+      <c r="G197" s="205"/>
+      <c r="H197" s="205"/>
+      <c r="I197" s="205"/>
+      <c r="J197" s="205"/>
+      <c r="K197" s="206"/>
     </row>
     <row r="198" spans="1:15">
       <c r="A198" s="12">
@@ -11017,16 +11022,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="186" t="s">
+      <c r="D198" s="204" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="187"/>
-      <c r="F198" s="187"/>
-      <c r="G198" s="187"/>
-      <c r="H198" s="187"/>
-      <c r="I198" s="187"/>
-      <c r="J198" s="187"/>
-      <c r="K198" s="188"/>
+      <c r="E198" s="205"/>
+      <c r="F198" s="205"/>
+      <c r="G198" s="205"/>
+      <c r="H198" s="205"/>
+      <c r="I198" s="205"/>
+      <c r="J198" s="205"/>
+      <c r="K198" s="206"/>
     </row>
     <row r="199" spans="1:15">
       <c r="A199" s="12">
@@ -11057,16 +11062,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="186" t="s">
+      <c r="D200" s="204" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="187"/>
-      <c r="F200" s="187"/>
-      <c r="G200" s="187"/>
-      <c r="H200" s="187"/>
-      <c r="I200" s="187"/>
-      <c r="J200" s="187"/>
-      <c r="K200" s="188"/>
+      <c r="E200" s="205"/>
+      <c r="F200" s="205"/>
+      <c r="G200" s="205"/>
+      <c r="H200" s="205"/>
+      <c r="I200" s="205"/>
+      <c r="J200" s="205"/>
+      <c r="K200" s="206"/>
     </row>
     <row r="201" spans="1:15">
       <c r="A201" s="12">
@@ -11097,16 +11102,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="216" t="s">
+      <c r="D202" s="210" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="217"/>
-      <c r="F202" s="217"/>
-      <c r="G202" s="217"/>
-      <c r="H202" s="217"/>
-      <c r="I202" s="217"/>
-      <c r="J202" s="217"/>
-      <c r="K202" s="218"/>
+      <c r="E202" s="211"/>
+      <c r="F202" s="211"/>
+      <c r="G202" s="211"/>
+      <c r="H202" s="211"/>
+      <c r="I202" s="211"/>
+      <c r="J202" s="211"/>
+      <c r="K202" s="212"/>
     </row>
     <row r="203" spans="1:15">
       <c r="A203" s="12">
@@ -11137,16 +11142,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="186" t="s">
+      <c r="D204" s="204" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="187"/>
-      <c r="F204" s="187"/>
-      <c r="G204" s="187"/>
-      <c r="H204" s="187"/>
-      <c r="I204" s="187"/>
-      <c r="J204" s="187"/>
-      <c r="K204" s="188"/>
+      <c r="E204" s="205"/>
+      <c r="F204" s="205"/>
+      <c r="G204" s="205"/>
+      <c r="H204" s="205"/>
+      <c r="I204" s="205"/>
+      <c r="J204" s="205"/>
+      <c r="K204" s="206"/>
     </row>
     <row r="205" spans="1:15">
       <c r="A205" s="12">
@@ -11177,16 +11182,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="186" t="s">
+      <c r="D206" s="204" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="187"/>
-      <c r="F206" s="187"/>
-      <c r="G206" s="187"/>
-      <c r="H206" s="187"/>
-      <c r="I206" s="187"/>
-      <c r="J206" s="187"/>
-      <c r="K206" s="188"/>
+      <c r="E206" s="205"/>
+      <c r="F206" s="205"/>
+      <c r="G206" s="205"/>
+      <c r="H206" s="205"/>
+      <c r="I206" s="205"/>
+      <c r="J206" s="205"/>
+      <c r="K206" s="206"/>
     </row>
     <row r="207" spans="1:15">
       <c r="A207" s="12">
@@ -11217,16 +11222,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="186" t="s">
+      <c r="D208" s="204" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="187"/>
-      <c r="F208" s="187"/>
-      <c r="G208" s="187"/>
-      <c r="H208" s="187"/>
-      <c r="I208" s="187"/>
-      <c r="J208" s="187"/>
-      <c r="K208" s="188"/>
+      <c r="E208" s="205"/>
+      <c r="F208" s="205"/>
+      <c r="G208" s="205"/>
+      <c r="H208" s="205"/>
+      <c r="I208" s="205"/>
+      <c r="J208" s="205"/>
+      <c r="K208" s="206"/>
     </row>
     <row r="209" spans="1:15" s="1" customFormat="1">
       <c r="A209" s="31">
@@ -11260,16 +11265,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="38"/>
-      <c r="D210" s="192" t="s">
+      <c r="D210" s="199" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="193"/>
-      <c r="F210" s="193"/>
-      <c r="G210" s="193"/>
-      <c r="H210" s="193"/>
-      <c r="I210" s="193"/>
-      <c r="J210" s="193"/>
-      <c r="K210" s="194"/>
+      <c r="E210" s="192"/>
+      <c r="F210" s="192"/>
+      <c r="G210" s="192"/>
+      <c r="H210" s="192"/>
+      <c r="I210" s="192"/>
+      <c r="J210" s="192"/>
+      <c r="K210" s="200"/>
     </row>
     <row r="211" spans="1:15">
       <c r="A211" s="12">
@@ -11338,16 +11343,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="186" t="s">
+      <c r="D214" s="204" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="187"/>
-      <c r="F214" s="187"/>
-      <c r="G214" s="187"/>
-      <c r="H214" s="187"/>
-      <c r="I214" s="187"/>
-      <c r="J214" s="187"/>
-      <c r="K214" s="188"/>
+      <c r="E214" s="205"/>
+      <c r="F214" s="205"/>
+      <c r="G214" s="205"/>
+      <c r="H214" s="205"/>
+      <c r="I214" s="205"/>
+      <c r="J214" s="205"/>
+      <c r="K214" s="206"/>
     </row>
     <row r="215" spans="1:15">
       <c r="A215" s="12">
@@ -11378,16 +11383,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="207" t="s">
+      <c r="D216" s="197" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="199"/>
-      <c r="F216" s="199"/>
-      <c r="G216" s="199"/>
-      <c r="H216" s="199"/>
-      <c r="I216" s="199"/>
-      <c r="J216" s="199"/>
-      <c r="K216" s="208"/>
+      <c r="E216" s="189"/>
+      <c r="F216" s="189"/>
+      <c r="G216" s="189"/>
+      <c r="H216" s="189"/>
+      <c r="I216" s="189"/>
+      <c r="J216" s="189"/>
+      <c r="K216" s="198"/>
     </row>
     <row r="217" spans="1:15">
       <c r="A217" s="12">
@@ -11399,14 +11404,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="192"/>
-      <c r="E217" s="193"/>
-      <c r="F217" s="193"/>
-      <c r="G217" s="193"/>
-      <c r="H217" s="193"/>
-      <c r="I217" s="193"/>
-      <c r="J217" s="193"/>
-      <c r="K217" s="194"/>
+      <c r="D217" s="199"/>
+      <c r="E217" s="192"/>
+      <c r="F217" s="192"/>
+      <c r="G217" s="192"/>
+      <c r="H217" s="192"/>
+      <c r="I217" s="192"/>
+      <c r="J217" s="192"/>
+      <c r="K217" s="200"/>
     </row>
     <row r="218" spans="1:15">
       <c r="A218" s="12">
@@ -11418,16 +11423,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="207" t="s">
+      <c r="D218" s="197" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="199"/>
-      <c r="F218" s="199"/>
-      <c r="G218" s="199"/>
-      <c r="H218" s="199"/>
-      <c r="I218" s="199"/>
-      <c r="J218" s="199"/>
-      <c r="K218" s="208"/>
+      <c r="E218" s="189"/>
+      <c r="F218" s="189"/>
+      <c r="G218" s="189"/>
+      <c r="H218" s="189"/>
+      <c r="I218" s="189"/>
+      <c r="J218" s="189"/>
+      <c r="K218" s="198"/>
     </row>
     <row r="219" spans="1:15">
       <c r="A219" s="12">
@@ -11439,14 +11444,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="192"/>
-      <c r="E219" s="193"/>
-      <c r="F219" s="193"/>
-      <c r="G219" s="193"/>
-      <c r="H219" s="193"/>
-      <c r="I219" s="193"/>
-      <c r="J219" s="193"/>
-      <c r="K219" s="194"/>
+      <c r="D219" s="199"/>
+      <c r="E219" s="192"/>
+      <c r="F219" s="192"/>
+      <c r="G219" s="192"/>
+      <c r="H219" s="192"/>
+      <c r="I219" s="192"/>
+      <c r="J219" s="192"/>
+      <c r="K219" s="200"/>
     </row>
     <row r="220" spans="1:15">
       <c r="A220" s="12">
@@ -11458,16 +11463,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="207" t="s">
+      <c r="D220" s="197" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="199"/>
-      <c r="F220" s="199"/>
-      <c r="G220" s="199"/>
-      <c r="H220" s="199"/>
-      <c r="I220" s="199"/>
-      <c r="J220" s="199"/>
-      <c r="K220" s="208"/>
+      <c r="E220" s="189"/>
+      <c r="F220" s="189"/>
+      <c r="G220" s="189"/>
+      <c r="H220" s="189"/>
+      <c r="I220" s="189"/>
+      <c r="J220" s="189"/>
+      <c r="K220" s="198"/>
     </row>
     <row r="221" spans="1:15">
       <c r="A221" s="12">
@@ -11479,14 +11484,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="192"/>
-      <c r="E221" s="193"/>
-      <c r="F221" s="193"/>
-      <c r="G221" s="193"/>
-      <c r="H221" s="193"/>
-      <c r="I221" s="193"/>
-      <c r="J221" s="193"/>
-      <c r="K221" s="194"/>
+      <c r="D221" s="199"/>
+      <c r="E221" s="192"/>
+      <c r="F221" s="192"/>
+      <c r="G221" s="192"/>
+      <c r="H221" s="192"/>
+      <c r="I221" s="192"/>
+      <c r="J221" s="192"/>
+      <c r="K221" s="200"/>
     </row>
     <row r="222" spans="1:15">
       <c r="A222" s="12">
@@ -11498,16 +11503,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="186" t="s">
+      <c r="D222" s="204" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="187"/>
-      <c r="F222" s="187"/>
-      <c r="G222" s="187"/>
-      <c r="H222" s="187"/>
-      <c r="I222" s="187"/>
-      <c r="J222" s="187"/>
-      <c r="K222" s="188"/>
+      <c r="E222" s="205"/>
+      <c r="F222" s="205"/>
+      <c r="G222" s="205"/>
+      <c r="H222" s="205"/>
+      <c r="I222" s="205"/>
+      <c r="J222" s="205"/>
+      <c r="K222" s="206"/>
     </row>
     <row r="223" spans="1:15">
       <c r="A223" s="12">
@@ -11538,16 +11543,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="186" t="s">
+      <c r="D224" s="204" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="187"/>
-      <c r="F224" s="187"/>
-      <c r="G224" s="187"/>
-      <c r="H224" s="187"/>
-      <c r="I224" s="187"/>
-      <c r="J224" s="187"/>
-      <c r="K224" s="188"/>
+      <c r="E224" s="205"/>
+      <c r="F224" s="205"/>
+      <c r="G224" s="205"/>
+      <c r="H224" s="205"/>
+      <c r="I224" s="205"/>
+      <c r="J224" s="205"/>
+      <c r="K224" s="206"/>
     </row>
     <row r="225" spans="1:15" s="1" customFormat="1">
       <c r="A225" s="31">
@@ -11581,16 +11586,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="38"/>
-      <c r="D226" s="213" t="s">
+      <c r="D226" s="207" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="214"/>
-      <c r="F226" s="214"/>
-      <c r="G226" s="214"/>
-      <c r="H226" s="214"/>
-      <c r="I226" s="214"/>
-      <c r="J226" s="214"/>
-      <c r="K226" s="215"/>
+      <c r="E226" s="208"/>
+      <c r="F226" s="208"/>
+      <c r="G226" s="208"/>
+      <c r="H226" s="208"/>
+      <c r="I226" s="208"/>
+      <c r="J226" s="208"/>
+      <c r="K226" s="209"/>
     </row>
     <row r="227" spans="1:15">
       <c r="A227" s="12">
@@ -11735,16 +11740,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="211" t="s">
+      <c r="D234" s="201" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="196"/>
-      <c r="F234" s="196"/>
-      <c r="G234" s="196"/>
-      <c r="H234" s="196"/>
-      <c r="I234" s="196"/>
-      <c r="J234" s="196"/>
-      <c r="K234" s="212"/>
+      <c r="E234" s="202"/>
+      <c r="F234" s="202"/>
+      <c r="G234" s="202"/>
+      <c r="H234" s="202"/>
+      <c r="I234" s="202"/>
+      <c r="J234" s="202"/>
+      <c r="K234" s="203"/>
     </row>
     <row r="235" spans="1:15">
       <c r="A235" s="12">
@@ -11813,16 +11818,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="203" t="s">
+      <c r="D238" s="188" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="199"/>
-      <c r="F238" s="199"/>
-      <c r="G238" s="199"/>
-      <c r="H238" s="199"/>
-      <c r="I238" s="199"/>
-      <c r="J238" s="199"/>
-      <c r="K238" s="200"/>
+      <c r="E238" s="189"/>
+      <c r="F238" s="189"/>
+      <c r="G238" s="189"/>
+      <c r="H238" s="189"/>
+      <c r="I238" s="189"/>
+      <c r="J238" s="189"/>
+      <c r="K238" s="190"/>
     </row>
     <row r="239" spans="1:15">
       <c r="A239" s="12">
@@ -11834,14 +11839,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="209"/>
-      <c r="E239" s="193"/>
-      <c r="F239" s="193"/>
-      <c r="G239" s="193"/>
-      <c r="H239" s="193"/>
-      <c r="I239" s="193"/>
-      <c r="J239" s="193"/>
-      <c r="K239" s="210"/>
+      <c r="D239" s="191"/>
+      <c r="E239" s="192"/>
+      <c r="F239" s="192"/>
+      <c r="G239" s="192"/>
+      <c r="H239" s="192"/>
+      <c r="I239" s="192"/>
+      <c r="J239" s="192"/>
+      <c r="K239" s="193"/>
     </row>
     <row r="240" spans="1:15">
       <c r="A240" s="12">
@@ -11853,16 +11858,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="68"/>
-      <c r="D240" s="199" t="s">
+      <c r="D240" s="189" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="199"/>
-      <c r="F240" s="199"/>
-      <c r="G240" s="199"/>
-      <c r="H240" s="199"/>
-      <c r="I240" s="199"/>
-      <c r="J240" s="199"/>
-      <c r="K240" s="200"/>
+      <c r="E240" s="189"/>
+      <c r="F240" s="189"/>
+      <c r="G240" s="189"/>
+      <c r="H240" s="189"/>
+      <c r="I240" s="189"/>
+      <c r="J240" s="189"/>
+      <c r="K240" s="190"/>
     </row>
     <row r="241" spans="1:15" s="1" customFormat="1">
       <c r="A241" s="31">
@@ -11874,14 +11879,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="33"/>
-      <c r="D241" s="201"/>
-      <c r="E241" s="201"/>
-      <c r="F241" s="201"/>
-      <c r="G241" s="201"/>
-      <c r="H241" s="201"/>
-      <c r="I241" s="201"/>
-      <c r="J241" s="201"/>
-      <c r="K241" s="202"/>
+      <c r="D241" s="216"/>
+      <c r="E241" s="216"/>
+      <c r="F241" s="216"/>
+      <c r="G241" s="216"/>
+      <c r="H241" s="216"/>
+      <c r="I241" s="216"/>
+      <c r="J241" s="216"/>
+      <c r="K241" s="217"/>
       <c r="M241" s="56"/>
       <c r="N241" s="57"/>
       <c r="O241" s="57"/>
@@ -12072,16 +12077,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="195" t="s">
+      <c r="D250" s="213" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="196"/>
-      <c r="F250" s="196"/>
-      <c r="G250" s="196"/>
-      <c r="H250" s="196"/>
-      <c r="I250" s="196"/>
-      <c r="J250" s="196"/>
-      <c r="K250" s="197"/>
+      <c r="E250" s="202"/>
+      <c r="F250" s="202"/>
+      <c r="G250" s="202"/>
+      <c r="H250" s="202"/>
+      <c r="I250" s="202"/>
+      <c r="J250" s="202"/>
+      <c r="K250" s="214"/>
     </row>
     <row r="251" spans="1:15">
       <c r="A251" s="12">
@@ -12650,16 +12655,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="198" t="s">
+      <c r="D280" s="215" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="187"/>
-      <c r="F280" s="187"/>
-      <c r="G280" s="187"/>
-      <c r="H280" s="187"/>
-      <c r="I280" s="187"/>
-      <c r="J280" s="187"/>
-      <c r="K280" s="188"/>
+      <c r="E280" s="205"/>
+      <c r="F280" s="205"/>
+      <c r="G280" s="205"/>
+      <c r="H280" s="205"/>
+      <c r="I280" s="205"/>
+      <c r="J280" s="205"/>
+      <c r="K280" s="206"/>
     </row>
     <row r="281" spans="1:15">
       <c r="A281" s="12">
@@ -12766,16 +12771,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="198" t="s">
+      <c r="D286" s="215" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="187"/>
-      <c r="F286" s="187"/>
-      <c r="G286" s="187"/>
-      <c r="H286" s="187"/>
-      <c r="I286" s="187"/>
-      <c r="J286" s="187"/>
-      <c r="K286" s="188"/>
+      <c r="E286" s="205"/>
+      <c r="F286" s="205"/>
+      <c r="G286" s="205"/>
+      <c r="H286" s="205"/>
+      <c r="I286" s="205"/>
+      <c r="J286" s="205"/>
+      <c r="K286" s="206"/>
     </row>
     <row r="287" spans="1:15">
       <c r="A287" s="12">
@@ -12963,16 +12968,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="186" t="s">
+      <c r="D296" s="204" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="187"/>
-      <c r="F296" s="187"/>
-      <c r="G296" s="187"/>
-      <c r="H296" s="187"/>
-      <c r="I296" s="187"/>
-      <c r="J296" s="187"/>
-      <c r="K296" s="188"/>
+      <c r="E296" s="205"/>
+      <c r="F296" s="205"/>
+      <c r="G296" s="205"/>
+      <c r="H296" s="205"/>
+      <c r="I296" s="205"/>
+      <c r="J296" s="205"/>
+      <c r="K296" s="206"/>
     </row>
     <row r="297" spans="1:15">
       <c r="A297" s="12">
@@ -13003,16 +13008,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="203" t="s">
+      <c r="D298" s="188" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="199"/>
-      <c r="F298" s="199"/>
-      <c r="G298" s="199"/>
-      <c r="H298" s="199"/>
-      <c r="I298" s="199"/>
-      <c r="J298" s="199"/>
-      <c r="K298" s="200"/>
+      <c r="E298" s="189"/>
+      <c r="F298" s="189"/>
+      <c r="G298" s="189"/>
+      <c r="H298" s="189"/>
+      <c r="I298" s="189"/>
+      <c r="J298" s="189"/>
+      <c r="K298" s="190"/>
     </row>
     <row r="299" spans="1:15">
       <c r="A299" s="12">
@@ -13024,14 +13029,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="209"/>
-      <c r="E299" s="193"/>
-      <c r="F299" s="193"/>
-      <c r="G299" s="193"/>
-      <c r="H299" s="193"/>
-      <c r="I299" s="193"/>
-      <c r="J299" s="193"/>
-      <c r="K299" s="210"/>
+      <c r="D299" s="191"/>
+      <c r="E299" s="192"/>
+      <c r="F299" s="192"/>
+      <c r="G299" s="192"/>
+      <c r="H299" s="192"/>
+      <c r="I299" s="192"/>
+      <c r="J299" s="192"/>
+      <c r="K299" s="193"/>
     </row>
     <row r="300" spans="1:15">
       <c r="A300" s="12">
@@ -13043,16 +13048,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="203" t="s">
+      <c r="D300" s="188" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="199"/>
-      <c r="F300" s="199"/>
-      <c r="G300" s="199"/>
-      <c r="H300" s="199"/>
-      <c r="I300" s="199"/>
-      <c r="J300" s="199"/>
-      <c r="K300" s="200"/>
+      <c r="E300" s="189"/>
+      <c r="F300" s="189"/>
+      <c r="G300" s="189"/>
+      <c r="H300" s="189"/>
+      <c r="I300" s="189"/>
+      <c r="J300" s="189"/>
+      <c r="K300" s="190"/>
     </row>
     <row r="301" spans="1:15">
       <c r="A301" s="12">
@@ -13064,14 +13069,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="209"/>
-      <c r="E301" s="193"/>
-      <c r="F301" s="193"/>
-      <c r="G301" s="193"/>
-      <c r="H301" s="193"/>
-      <c r="I301" s="193"/>
-      <c r="J301" s="193"/>
-      <c r="K301" s="210"/>
+      <c r="D301" s="191"/>
+      <c r="E301" s="192"/>
+      <c r="F301" s="192"/>
+      <c r="G301" s="192"/>
+      <c r="H301" s="192"/>
+      <c r="I301" s="192"/>
+      <c r="J301" s="192"/>
+      <c r="K301" s="193"/>
     </row>
     <row r="302" spans="1:15">
       <c r="A302" s="12">
@@ -13083,16 +13088,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="203" t="s">
+      <c r="D302" s="188" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="199"/>
-      <c r="F302" s="199"/>
-      <c r="G302" s="199"/>
-      <c r="H302" s="199"/>
-      <c r="I302" s="199"/>
-      <c r="J302" s="199"/>
-      <c r="K302" s="200"/>
+      <c r="E302" s="189"/>
+      <c r="F302" s="189"/>
+      <c r="G302" s="189"/>
+      <c r="H302" s="189"/>
+      <c r="I302" s="189"/>
+      <c r="J302" s="189"/>
+      <c r="K302" s="190"/>
     </row>
     <row r="303" spans="1:15">
       <c r="A303" s="12">
@@ -13104,14 +13109,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="209"/>
-      <c r="E303" s="193"/>
-      <c r="F303" s="193"/>
-      <c r="G303" s="193"/>
-      <c r="H303" s="193"/>
-      <c r="I303" s="193"/>
-      <c r="J303" s="193"/>
-      <c r="K303" s="210"/>
+      <c r="D303" s="191"/>
+      <c r="E303" s="192"/>
+      <c r="F303" s="192"/>
+      <c r="G303" s="192"/>
+      <c r="H303" s="192"/>
+      <c r="I303" s="192"/>
+      <c r="J303" s="192"/>
+      <c r="K303" s="193"/>
     </row>
     <row r="304" spans="1:15">
       <c r="A304" s="12">
@@ -13123,16 +13128,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="203" t="s">
+      <c r="D304" s="188" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="199"/>
-      <c r="F304" s="199"/>
-      <c r="G304" s="199"/>
-      <c r="H304" s="199"/>
-      <c r="I304" s="199"/>
-      <c r="J304" s="199"/>
-      <c r="K304" s="200"/>
+      <c r="E304" s="189"/>
+      <c r="F304" s="189"/>
+      <c r="G304" s="189"/>
+      <c r="H304" s="189"/>
+      <c r="I304" s="189"/>
+      <c r="J304" s="189"/>
+      <c r="K304" s="190"/>
     </row>
     <row r="305" spans="1:15" s="1" customFormat="1">
       <c r="A305" s="31">
@@ -13144,14 +13149,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="32"/>
-      <c r="D305" s="209"/>
-      <c r="E305" s="193"/>
-      <c r="F305" s="193"/>
-      <c r="G305" s="193"/>
-      <c r="H305" s="193"/>
-      <c r="I305" s="193"/>
-      <c r="J305" s="193"/>
-      <c r="K305" s="210"/>
+      <c r="D305" s="191"/>
+      <c r="E305" s="192"/>
+      <c r="F305" s="192"/>
+      <c r="G305" s="192"/>
+      <c r="H305" s="192"/>
+      <c r="I305" s="192"/>
+      <c r="J305" s="192"/>
+      <c r="K305" s="193"/>
       <c r="M305" s="56"/>
       <c r="N305" s="57"/>
       <c r="O305" s="57"/>
@@ -13166,16 +13171,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="38"/>
-      <c r="D306" s="203" t="s">
+      <c r="D306" s="188" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="199"/>
-      <c r="F306" s="199"/>
-      <c r="G306" s="199"/>
-      <c r="H306" s="199"/>
-      <c r="I306" s="199"/>
-      <c r="J306" s="199"/>
-      <c r="K306" s="200"/>
+      <c r="E306" s="189"/>
+      <c r="F306" s="189"/>
+      <c r="G306" s="189"/>
+      <c r="H306" s="189"/>
+      <c r="I306" s="189"/>
+      <c r="J306" s="189"/>
+      <c r="K306" s="190"/>
     </row>
     <row r="307" spans="1:15">
       <c r="A307" s="12">
@@ -13187,14 +13192,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="209"/>
-      <c r="E307" s="193"/>
-      <c r="F307" s="193"/>
-      <c r="G307" s="193"/>
-      <c r="H307" s="193"/>
-      <c r="I307" s="193"/>
-      <c r="J307" s="193"/>
-      <c r="K307" s="210"/>
+      <c r="D307" s="191"/>
+      <c r="E307" s="192"/>
+      <c r="F307" s="192"/>
+      <c r="G307" s="192"/>
+      <c r="H307" s="192"/>
+      <c r="I307" s="192"/>
+      <c r="J307" s="192"/>
+      <c r="K307" s="193"/>
     </row>
     <row r="308" spans="1:15">
       <c r="A308" s="12">
@@ -13206,16 +13211,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="203" t="s">
+      <c r="D308" s="188" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="199"/>
-      <c r="F308" s="199"/>
-      <c r="G308" s="199"/>
-      <c r="H308" s="199"/>
-      <c r="I308" s="199"/>
-      <c r="J308" s="199"/>
-      <c r="K308" s="200"/>
+      <c r="E308" s="189"/>
+      <c r="F308" s="189"/>
+      <c r="G308" s="189"/>
+      <c r="H308" s="189"/>
+      <c r="I308" s="189"/>
+      <c r="J308" s="189"/>
+      <c r="K308" s="190"/>
     </row>
     <row r="309" spans="1:15">
       <c r="A309" s="12">
@@ -13227,14 +13232,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="209"/>
-      <c r="E309" s="193"/>
-      <c r="F309" s="193"/>
-      <c r="G309" s="193"/>
-      <c r="H309" s="193"/>
-      <c r="I309" s="193"/>
-      <c r="J309" s="193"/>
-      <c r="K309" s="210"/>
+      <c r="D309" s="191"/>
+      <c r="E309" s="192"/>
+      <c r="F309" s="192"/>
+      <c r="G309" s="192"/>
+      <c r="H309" s="192"/>
+      <c r="I309" s="192"/>
+      <c r="J309" s="192"/>
+      <c r="K309" s="193"/>
     </row>
     <row r="310" spans="1:15">
       <c r="A310" s="12">
@@ -21521,16 +21526,16 @@
         <f t="shared" si="35"/>
         <v>DB8</v>
       </c>
-      <c r="D954" s="219" t="s">
+      <c r="D954" s="186" t="s">
         <v>480</v>
       </c>
-      <c r="E954" s="220"/>
-      <c r="F954" s="220"/>
-      <c r="G954" s="220"/>
-      <c r="H954" s="220"/>
-      <c r="I954" s="220"/>
-      <c r="J954" s="220"/>
-      <c r="K954" s="220"/>
+      <c r="E954" s="187"/>
+      <c r="F954" s="187"/>
+      <c r="G954" s="187"/>
+      <c r="H954" s="187"/>
+      <c r="I954" s="187"/>
+      <c r="J954" s="187"/>
+      <c r="K954" s="187"/>
     </row>
     <row r="955" spans="1:11">
       <c r="A955" s="12">
@@ -24364,13 +24369,31 @@
     </row>
   </sheetData>
   <mergeCells count="48">
-    <mergeCell ref="D954:K954"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D168:K168"/>
+    <mergeCell ref="D175:K175"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D250:K250"/>
+    <mergeCell ref="D280:K280"/>
+    <mergeCell ref="D286:K286"/>
+    <mergeCell ref="D296:K296"/>
+    <mergeCell ref="D240:K241"/>
     <mergeCell ref="D2:K3"/>
     <mergeCell ref="D216:K217"/>
     <mergeCell ref="D218:K219"/>
@@ -24387,31 +24410,13 @@
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
     <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D250:K250"/>
-    <mergeCell ref="D280:K280"/>
-    <mergeCell ref="D286:K286"/>
-    <mergeCell ref="D296:K296"/>
-    <mergeCell ref="D240:K241"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D168:K168"/>
-    <mergeCell ref="D175:K175"/>
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D954:K954"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -24497,16 +24502,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="203" t="s">
+      <c r="D2" s="188" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="199"/>
-      <c r="F2" s="199"/>
-      <c r="G2" s="199"/>
-      <c r="H2" s="199"/>
-      <c r="I2" s="199"/>
-      <c r="J2" s="199"/>
-      <c r="K2" s="200"/>
+      <c r="E2" s="189"/>
+      <c r="F2" s="189"/>
+      <c r="G2" s="189"/>
+      <c r="H2" s="189"/>
+      <c r="I2" s="189"/>
+      <c r="J2" s="189"/>
+      <c r="K2" s="190"/>
       <c r="M2" s="3">
         <v>16</v>
       </c>
@@ -24528,14 +24533,14 @@
         <f t="shared" ref="C3:C33" si="2">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="209"/>
-      <c r="E3" s="193"/>
-      <c r="F3" s="193"/>
-      <c r="G3" s="193"/>
-      <c r="H3" s="193"/>
-      <c r="I3" s="193"/>
-      <c r="J3" s="193"/>
-      <c r="K3" s="206"/>
+      <c r="D3" s="191"/>
+      <c r="E3" s="192"/>
+      <c r="F3" s="192"/>
+      <c r="G3" s="192"/>
+      <c r="H3" s="192"/>
+      <c r="I3" s="192"/>
+      <c r="J3" s="192"/>
+      <c r="K3" s="196"/>
       <c r="M3" s="3">
         <v>17</v>
       </c>
@@ -30784,16 +30789,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="38"/>
-      <c r="D178" s="184" t="s">
+      <c r="D178" s="221" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="184"/>
-      <c r="F178" s="184"/>
-      <c r="G178" s="184"/>
-      <c r="H178" s="184"/>
-      <c r="I178" s="184"/>
-      <c r="J178" s="184"/>
-      <c r="K178" s="184"/>
+      <c r="E178" s="221"/>
+      <c r="F178" s="221"/>
+      <c r="G178" s="221"/>
+      <c r="H178" s="221"/>
+      <c r="I178" s="221"/>
+      <c r="J178" s="221"/>
+      <c r="K178" s="221"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -30862,16 +30867,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="186" t="s">
+      <c r="D182" s="204" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="187"/>
-      <c r="F182" s="187"/>
-      <c r="G182" s="187"/>
-      <c r="H182" s="187"/>
-      <c r="I182" s="187"/>
-      <c r="J182" s="187"/>
-      <c r="K182" s="188"/>
+      <c r="E182" s="205"/>
+      <c r="F182" s="205"/>
+      <c r="G182" s="205"/>
+      <c r="H182" s="205"/>
+      <c r="I182" s="205"/>
+      <c r="J182" s="205"/>
+      <c r="K182" s="206"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -30883,16 +30888,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="186" t="s">
+      <c r="D183" s="204" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="187"/>
-      <c r="F183" s="187"/>
-      <c r="G183" s="187"/>
-      <c r="H183" s="187"/>
-      <c r="I183" s="187"/>
-      <c r="J183" s="187"/>
-      <c r="K183" s="188"/>
+      <c r="E183" s="205"/>
+      <c r="F183" s="205"/>
+      <c r="G183" s="205"/>
+      <c r="H183" s="205"/>
+      <c r="I183" s="205"/>
+      <c r="J183" s="205"/>
+      <c r="K183" s="206"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -30904,16 +30909,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="186" t="s">
+      <c r="D184" s="204" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="187"/>
-      <c r="F184" s="187"/>
-      <c r="G184" s="187"/>
-      <c r="H184" s="187"/>
-      <c r="I184" s="187"/>
-      <c r="J184" s="187"/>
-      <c r="K184" s="188"/>
+      <c r="E184" s="205"/>
+      <c r="F184" s="205"/>
+      <c r="G184" s="205"/>
+      <c r="H184" s="205"/>
+      <c r="I184" s="205"/>
+      <c r="J184" s="205"/>
+      <c r="K184" s="206"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -30925,16 +30930,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="186" t="s">
+      <c r="D185" s="204" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="187"/>
-      <c r="F185" s="187"/>
-      <c r="G185" s="187"/>
-      <c r="H185" s="187"/>
-      <c r="I185" s="187"/>
-      <c r="J185" s="187"/>
-      <c r="K185" s="188"/>
+      <c r="E185" s="205"/>
+      <c r="F185" s="205"/>
+      <c r="G185" s="205"/>
+      <c r="H185" s="205"/>
+      <c r="I185" s="205"/>
+      <c r="J185" s="205"/>
+      <c r="K185" s="206"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -30946,16 +30951,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="186" t="s">
+      <c r="D186" s="204" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="187"/>
-      <c r="F186" s="187"/>
-      <c r="G186" s="187"/>
-      <c r="H186" s="187"/>
-      <c r="I186" s="187"/>
-      <c r="J186" s="187"/>
-      <c r="K186" s="188"/>
+      <c r="E186" s="205"/>
+      <c r="F186" s="205"/>
+      <c r="G186" s="205"/>
+      <c r="H186" s="205"/>
+      <c r="I186" s="205"/>
+      <c r="J186" s="205"/>
+      <c r="K186" s="206"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -30967,16 +30972,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="186" t="s">
+      <c r="D187" s="204" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="187"/>
-      <c r="F187" s="187"/>
-      <c r="G187" s="187"/>
-      <c r="H187" s="187"/>
-      <c r="I187" s="187"/>
-      <c r="J187" s="187"/>
-      <c r="K187" s="188"/>
+      <c r="E187" s="205"/>
+      <c r="F187" s="205"/>
+      <c r="G187" s="205"/>
+      <c r="H187" s="205"/>
+      <c r="I187" s="205"/>
+      <c r="J187" s="205"/>
+      <c r="K187" s="206"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -30988,16 +30993,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="186" t="s">
+      <c r="D188" s="204" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="187"/>
-      <c r="F188" s="187"/>
-      <c r="G188" s="187"/>
-      <c r="H188" s="187"/>
-      <c r="I188" s="187"/>
-      <c r="J188" s="187"/>
-      <c r="K188" s="188"/>
+      <c r="E188" s="205"/>
+      <c r="F188" s="205"/>
+      <c r="G188" s="205"/>
+      <c r="H188" s="205"/>
+      <c r="I188" s="205"/>
+      <c r="J188" s="205"/>
+      <c r="K188" s="206"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -31009,16 +31014,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="186" t="s">
+      <c r="D189" s="204" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="187"/>
-      <c r="F189" s="187"/>
-      <c r="G189" s="187"/>
-      <c r="H189" s="187"/>
-      <c r="I189" s="187"/>
-      <c r="J189" s="187"/>
-      <c r="K189" s="188"/>
+      <c r="E189" s="205"/>
+      <c r="F189" s="205"/>
+      <c r="G189" s="205"/>
+      <c r="H189" s="205"/>
+      <c r="I189" s="205"/>
+      <c r="J189" s="205"/>
+      <c r="K189" s="206"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -31030,16 +31035,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="186" t="s">
+      <c r="D190" s="204" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="187"/>
-      <c r="F190" s="187"/>
-      <c r="G190" s="187"/>
-      <c r="H190" s="187"/>
-      <c r="I190" s="187"/>
-      <c r="J190" s="187"/>
-      <c r="K190" s="188"/>
+      <c r="E190" s="205"/>
+      <c r="F190" s="205"/>
+      <c r="G190" s="205"/>
+      <c r="H190" s="205"/>
+      <c r="I190" s="205"/>
+      <c r="J190" s="205"/>
+      <c r="K190" s="206"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -31051,16 +31056,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="186" t="s">
+      <c r="D191" s="204" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="187"/>
-      <c r="F191" s="187"/>
-      <c r="G191" s="187"/>
-      <c r="H191" s="187"/>
-      <c r="I191" s="187"/>
-      <c r="J191" s="187"/>
-      <c r="K191" s="188"/>
+      <c r="E191" s="205"/>
+      <c r="F191" s="205"/>
+      <c r="G191" s="205"/>
+      <c r="H191" s="205"/>
+      <c r="I191" s="205"/>
+      <c r="J191" s="205"/>
+      <c r="K191" s="206"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -31072,16 +31077,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="186" t="s">
+      <c r="D192" s="204" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="187"/>
-      <c r="F192" s="187"/>
-      <c r="G192" s="187"/>
-      <c r="H192" s="187"/>
-      <c r="I192" s="187"/>
-      <c r="J192" s="187"/>
-      <c r="K192" s="188"/>
+      <c r="E192" s="205"/>
+      <c r="F192" s="205"/>
+      <c r="G192" s="205"/>
+      <c r="H192" s="205"/>
+      <c r="I192" s="205"/>
+      <c r="J192" s="205"/>
+      <c r="K192" s="206"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="31">
@@ -31093,16 +31098,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="32"/>
-      <c r="D193" s="189" t="s">
+      <c r="D193" s="218" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="190"/>
-      <c r="F193" s="190"/>
-      <c r="G193" s="190"/>
-      <c r="H193" s="190"/>
-      <c r="I193" s="190"/>
-      <c r="J193" s="190"/>
-      <c r="K193" s="191"/>
+      <c r="E193" s="219"/>
+      <c r="F193" s="219"/>
+      <c r="G193" s="219"/>
+      <c r="H193" s="219"/>
+      <c r="I193" s="219"/>
+      <c r="J193" s="219"/>
+      <c r="K193" s="220"/>
       <c r="L193" s="56"/>
       <c r="M193" s="57"/>
       <c r="N193" s="57"/>
@@ -31117,16 +31122,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="38"/>
-      <c r="D194" s="192" t="s">
+      <c r="D194" s="199" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="193"/>
-      <c r="F194" s="193"/>
-      <c r="G194" s="193"/>
-      <c r="H194" s="193"/>
-      <c r="I194" s="193"/>
-      <c r="J194" s="193"/>
-      <c r="K194" s="194"/>
+      <c r="E194" s="192"/>
+      <c r="F194" s="192"/>
+      <c r="G194" s="192"/>
+      <c r="H194" s="192"/>
+      <c r="I194" s="192"/>
+      <c r="J194" s="192"/>
+      <c r="K194" s="200"/>
     </row>
     <row r="195" spans="1:14">
       <c r="A195" s="12">
@@ -31138,16 +31143,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="186" t="s">
+      <c r="D195" s="204" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="187"/>
-      <c r="F195" s="187"/>
-      <c r="G195" s="187"/>
-      <c r="H195" s="187"/>
-      <c r="I195" s="187"/>
-      <c r="J195" s="187"/>
-      <c r="K195" s="188"/>
+      <c r="E195" s="205"/>
+      <c r="F195" s="205"/>
+      <c r="G195" s="205"/>
+      <c r="H195" s="205"/>
+      <c r="I195" s="205"/>
+      <c r="J195" s="205"/>
+      <c r="K195" s="206"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -31159,16 +31164,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="186" t="s">
+      <c r="D196" s="204" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="187"/>
-      <c r="F196" s="187"/>
-      <c r="G196" s="187"/>
-      <c r="H196" s="187"/>
-      <c r="I196" s="187"/>
-      <c r="J196" s="187"/>
-      <c r="K196" s="188"/>
+      <c r="E196" s="205"/>
+      <c r="F196" s="205"/>
+      <c r="G196" s="205"/>
+      <c r="H196" s="205"/>
+      <c r="I196" s="205"/>
+      <c r="J196" s="205"/>
+      <c r="K196" s="206"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -31180,16 +31185,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="186" t="s">
+      <c r="D197" s="204" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="187"/>
-      <c r="F197" s="187"/>
-      <c r="G197" s="187"/>
-      <c r="H197" s="187"/>
-      <c r="I197" s="187"/>
-      <c r="J197" s="187"/>
-      <c r="K197" s="188"/>
+      <c r="E197" s="205"/>
+      <c r="F197" s="205"/>
+      <c r="G197" s="205"/>
+      <c r="H197" s="205"/>
+      <c r="I197" s="205"/>
+      <c r="J197" s="205"/>
+      <c r="K197" s="206"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -31201,16 +31206,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="186" t="s">
+      <c r="D198" s="204" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="187"/>
-      <c r="F198" s="187"/>
-      <c r="G198" s="187"/>
-      <c r="H198" s="187"/>
-      <c r="I198" s="187"/>
-      <c r="J198" s="187"/>
-      <c r="K198" s="188"/>
+      <c r="E198" s="205"/>
+      <c r="F198" s="205"/>
+      <c r="G198" s="205"/>
+      <c r="H198" s="205"/>
+      <c r="I198" s="205"/>
+      <c r="J198" s="205"/>
+      <c r="K198" s="206"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -31241,16 +31246,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="186" t="s">
+      <c r="D200" s="204" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="187"/>
-      <c r="F200" s="187"/>
-      <c r="G200" s="187"/>
-      <c r="H200" s="187"/>
-      <c r="I200" s="187"/>
-      <c r="J200" s="187"/>
-      <c r="K200" s="188"/>
+      <c r="E200" s="205"/>
+      <c r="F200" s="205"/>
+      <c r="G200" s="205"/>
+      <c r="H200" s="205"/>
+      <c r="I200" s="205"/>
+      <c r="J200" s="205"/>
+      <c r="K200" s="206"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -31281,16 +31286,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="216" t="s">
+      <c r="D202" s="210" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="217"/>
-      <c r="F202" s="217"/>
-      <c r="G202" s="217"/>
-      <c r="H202" s="217"/>
-      <c r="I202" s="217"/>
-      <c r="J202" s="217"/>
-      <c r="K202" s="218"/>
+      <c r="E202" s="211"/>
+      <c r="F202" s="211"/>
+      <c r="G202" s="211"/>
+      <c r="H202" s="211"/>
+      <c r="I202" s="211"/>
+      <c r="J202" s="211"/>
+      <c r="K202" s="212"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -31321,16 +31326,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="186" t="s">
+      <c r="D204" s="204" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="187"/>
-      <c r="F204" s="187"/>
-      <c r="G204" s="187"/>
-      <c r="H204" s="187"/>
-      <c r="I204" s="187"/>
-      <c r="J204" s="187"/>
-      <c r="K204" s="188"/>
+      <c r="E204" s="205"/>
+      <c r="F204" s="205"/>
+      <c r="G204" s="205"/>
+      <c r="H204" s="205"/>
+      <c r="I204" s="205"/>
+      <c r="J204" s="205"/>
+      <c r="K204" s="206"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -31361,16 +31366,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="186" t="s">
+      <c r="D206" s="204" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="187"/>
-      <c r="F206" s="187"/>
-      <c r="G206" s="187"/>
-      <c r="H206" s="187"/>
-      <c r="I206" s="187"/>
-      <c r="J206" s="187"/>
-      <c r="K206" s="188"/>
+      <c r="E206" s="205"/>
+      <c r="F206" s="205"/>
+      <c r="G206" s="205"/>
+      <c r="H206" s="205"/>
+      <c r="I206" s="205"/>
+      <c r="J206" s="205"/>
+      <c r="K206" s="206"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -31401,16 +31406,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="186" t="s">
+      <c r="D208" s="204" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="187"/>
-      <c r="F208" s="187"/>
-      <c r="G208" s="187"/>
-      <c r="H208" s="187"/>
-      <c r="I208" s="187"/>
-      <c r="J208" s="187"/>
-      <c r="K208" s="188"/>
+      <c r="E208" s="205"/>
+      <c r="F208" s="205"/>
+      <c r="G208" s="205"/>
+      <c r="H208" s="205"/>
+      <c r="I208" s="205"/>
+      <c r="J208" s="205"/>
+      <c r="K208" s="206"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="31">
@@ -31444,16 +31449,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="38"/>
-      <c r="D210" s="192" t="s">
+      <c r="D210" s="199" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="193"/>
-      <c r="F210" s="193"/>
-      <c r="G210" s="193"/>
-      <c r="H210" s="193"/>
-      <c r="I210" s="193"/>
-      <c r="J210" s="193"/>
-      <c r="K210" s="194"/>
+      <c r="E210" s="192"/>
+      <c r="F210" s="192"/>
+      <c r="G210" s="192"/>
+      <c r="H210" s="192"/>
+      <c r="I210" s="192"/>
+      <c r="J210" s="192"/>
+      <c r="K210" s="200"/>
     </row>
     <row r="211" spans="1:14">
       <c r="A211" s="12">
@@ -31522,16 +31527,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="186" t="s">
+      <c r="D214" s="204" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="187"/>
-      <c r="F214" s="187"/>
-      <c r="G214" s="187"/>
-      <c r="H214" s="187"/>
-      <c r="I214" s="187"/>
-      <c r="J214" s="187"/>
-      <c r="K214" s="188"/>
+      <c r="E214" s="205"/>
+      <c r="F214" s="205"/>
+      <c r="G214" s="205"/>
+      <c r="H214" s="205"/>
+      <c r="I214" s="205"/>
+      <c r="J214" s="205"/>
+      <c r="K214" s="206"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -31562,16 +31567,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="207" t="s">
+      <c r="D216" s="197" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="199"/>
-      <c r="F216" s="199"/>
-      <c r="G216" s="199"/>
-      <c r="H216" s="199"/>
-      <c r="I216" s="199"/>
-      <c r="J216" s="199"/>
-      <c r="K216" s="208"/>
+      <c r="E216" s="189"/>
+      <c r="F216" s="189"/>
+      <c r="G216" s="189"/>
+      <c r="H216" s="189"/>
+      <c r="I216" s="189"/>
+      <c r="J216" s="189"/>
+      <c r="K216" s="198"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -31583,14 +31588,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="192"/>
-      <c r="E217" s="193"/>
-      <c r="F217" s="193"/>
-      <c r="G217" s="193"/>
-      <c r="H217" s="193"/>
-      <c r="I217" s="193"/>
-      <c r="J217" s="193"/>
-      <c r="K217" s="194"/>
+      <c r="D217" s="199"/>
+      <c r="E217" s="192"/>
+      <c r="F217" s="192"/>
+      <c r="G217" s="192"/>
+      <c r="H217" s="192"/>
+      <c r="I217" s="192"/>
+      <c r="J217" s="192"/>
+      <c r="K217" s="200"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="12">
@@ -31602,16 +31607,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="207" t="s">
+      <c r="D218" s="197" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="199"/>
-      <c r="F218" s="199"/>
-      <c r="G218" s="199"/>
-      <c r="H218" s="199"/>
-      <c r="I218" s="199"/>
-      <c r="J218" s="199"/>
-      <c r="K218" s="208"/>
+      <c r="E218" s="189"/>
+      <c r="F218" s="189"/>
+      <c r="G218" s="189"/>
+      <c r="H218" s="189"/>
+      <c r="I218" s="189"/>
+      <c r="J218" s="189"/>
+      <c r="K218" s="198"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -31623,14 +31628,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="192"/>
-      <c r="E219" s="193"/>
-      <c r="F219" s="193"/>
-      <c r="G219" s="193"/>
-      <c r="H219" s="193"/>
-      <c r="I219" s="193"/>
-      <c r="J219" s="193"/>
-      <c r="K219" s="194"/>
+      <c r="D219" s="199"/>
+      <c r="E219" s="192"/>
+      <c r="F219" s="192"/>
+      <c r="G219" s="192"/>
+      <c r="H219" s="192"/>
+      <c r="I219" s="192"/>
+      <c r="J219" s="192"/>
+      <c r="K219" s="200"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="12">
@@ -31642,16 +31647,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="207" t="s">
+      <c r="D220" s="197" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="199"/>
-      <c r="F220" s="199"/>
-      <c r="G220" s="199"/>
-      <c r="H220" s="199"/>
-      <c r="I220" s="199"/>
-      <c r="J220" s="199"/>
-      <c r="K220" s="208"/>
+      <c r="E220" s="189"/>
+      <c r="F220" s="189"/>
+      <c r="G220" s="189"/>
+      <c r="H220" s="189"/>
+      <c r="I220" s="189"/>
+      <c r="J220" s="189"/>
+      <c r="K220" s="198"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -31663,14 +31668,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="192"/>
-      <c r="E221" s="193"/>
-      <c r="F221" s="193"/>
-      <c r="G221" s="193"/>
-      <c r="H221" s="193"/>
-      <c r="I221" s="193"/>
-      <c r="J221" s="193"/>
-      <c r="K221" s="194"/>
+      <c r="D221" s="199"/>
+      <c r="E221" s="192"/>
+      <c r="F221" s="192"/>
+      <c r="G221" s="192"/>
+      <c r="H221" s="192"/>
+      <c r="I221" s="192"/>
+      <c r="J221" s="192"/>
+      <c r="K221" s="200"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="12">
@@ -31682,16 +31687,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="186" t="s">
+      <c r="D222" s="204" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="187"/>
-      <c r="F222" s="187"/>
-      <c r="G222" s="187"/>
-      <c r="H222" s="187"/>
-      <c r="I222" s="187"/>
-      <c r="J222" s="187"/>
-      <c r="K222" s="188"/>
+      <c r="E222" s="205"/>
+      <c r="F222" s="205"/>
+      <c r="G222" s="205"/>
+      <c r="H222" s="205"/>
+      <c r="I222" s="205"/>
+      <c r="J222" s="205"/>
+      <c r="K222" s="206"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -31722,16 +31727,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="186" t="s">
+      <c r="D224" s="204" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="187"/>
-      <c r="F224" s="187"/>
-      <c r="G224" s="187"/>
-      <c r="H224" s="187"/>
-      <c r="I224" s="187"/>
-      <c r="J224" s="187"/>
-      <c r="K224" s="188"/>
+      <c r="E224" s="205"/>
+      <c r="F224" s="205"/>
+      <c r="G224" s="205"/>
+      <c r="H224" s="205"/>
+      <c r="I224" s="205"/>
+      <c r="J224" s="205"/>
+      <c r="K224" s="206"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="31">
@@ -31765,16 +31770,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="38"/>
-      <c r="D226" s="213" t="s">
+      <c r="D226" s="207" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="214"/>
-      <c r="F226" s="214"/>
-      <c r="G226" s="214"/>
-      <c r="H226" s="214"/>
-      <c r="I226" s="214"/>
-      <c r="J226" s="214"/>
-      <c r="K226" s="215"/>
+      <c r="E226" s="208"/>
+      <c r="F226" s="208"/>
+      <c r="G226" s="208"/>
+      <c r="H226" s="208"/>
+      <c r="I226" s="208"/>
+      <c r="J226" s="208"/>
+      <c r="K226" s="209"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -31919,16 +31924,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="211" t="s">
+      <c r="D234" s="201" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="196"/>
-      <c r="F234" s="196"/>
-      <c r="G234" s="196"/>
-      <c r="H234" s="196"/>
-      <c r="I234" s="196"/>
-      <c r="J234" s="196"/>
-      <c r="K234" s="212"/>
+      <c r="E234" s="202"/>
+      <c r="F234" s="202"/>
+      <c r="G234" s="202"/>
+      <c r="H234" s="202"/>
+      <c r="I234" s="202"/>
+      <c r="J234" s="202"/>
+      <c r="K234" s="203"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -31997,16 +32002,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="203" t="s">
+      <c r="D238" s="188" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="199"/>
-      <c r="F238" s="199"/>
-      <c r="G238" s="199"/>
-      <c r="H238" s="199"/>
-      <c r="I238" s="199"/>
-      <c r="J238" s="199"/>
-      <c r="K238" s="200"/>
+      <c r="E238" s="189"/>
+      <c r="F238" s="189"/>
+      <c r="G238" s="189"/>
+      <c r="H238" s="189"/>
+      <c r="I238" s="189"/>
+      <c r="J238" s="189"/>
+      <c r="K238" s="190"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -32018,14 +32023,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="209"/>
-      <c r="E239" s="193"/>
-      <c r="F239" s="193"/>
-      <c r="G239" s="193"/>
-      <c r="H239" s="193"/>
-      <c r="I239" s="193"/>
-      <c r="J239" s="193"/>
-      <c r="K239" s="210"/>
+      <c r="D239" s="191"/>
+      <c r="E239" s="192"/>
+      <c r="F239" s="192"/>
+      <c r="G239" s="192"/>
+      <c r="H239" s="192"/>
+      <c r="I239" s="192"/>
+      <c r="J239" s="192"/>
+      <c r="K239" s="193"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -32037,16 +32042,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="68"/>
-      <c r="D240" s="199" t="s">
+      <c r="D240" s="189" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="199"/>
-      <c r="F240" s="199"/>
-      <c r="G240" s="199"/>
-      <c r="H240" s="199"/>
-      <c r="I240" s="199"/>
-      <c r="J240" s="199"/>
-      <c r="K240" s="200"/>
+      <c r="E240" s="189"/>
+      <c r="F240" s="189"/>
+      <c r="G240" s="189"/>
+      <c r="H240" s="189"/>
+      <c r="I240" s="189"/>
+      <c r="J240" s="189"/>
+      <c r="K240" s="190"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="31">
@@ -32058,14 +32063,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="33"/>
-      <c r="D241" s="201"/>
-      <c r="E241" s="201"/>
-      <c r="F241" s="201"/>
-      <c r="G241" s="201"/>
-      <c r="H241" s="201"/>
-      <c r="I241" s="201"/>
-      <c r="J241" s="201"/>
-      <c r="K241" s="202"/>
+      <c r="D241" s="216"/>
+      <c r="E241" s="216"/>
+      <c r="F241" s="216"/>
+      <c r="G241" s="216"/>
+      <c r="H241" s="216"/>
+      <c r="I241" s="216"/>
+      <c r="J241" s="216"/>
+      <c r="K241" s="217"/>
       <c r="L241" s="56"/>
       <c r="M241" s="57"/>
       <c r="N241" s="57"/>
@@ -32256,16 +32261,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="195" t="s">
+      <c r="D250" s="213" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="196"/>
-      <c r="F250" s="196"/>
-      <c r="G250" s="196"/>
-      <c r="H250" s="196"/>
-      <c r="I250" s="196"/>
-      <c r="J250" s="196"/>
-      <c r="K250" s="197"/>
+      <c r="E250" s="202"/>
+      <c r="F250" s="202"/>
+      <c r="G250" s="202"/>
+      <c r="H250" s="202"/>
+      <c r="I250" s="202"/>
+      <c r="J250" s="202"/>
+      <c r="K250" s="214"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -32834,16 +32839,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="186" t="s">
+      <c r="D280" s="204" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="187"/>
-      <c r="F280" s="187"/>
-      <c r="G280" s="187"/>
-      <c r="H280" s="187"/>
-      <c r="I280" s="187"/>
-      <c r="J280" s="187"/>
-      <c r="K280" s="188"/>
+      <c r="E280" s="205"/>
+      <c r="F280" s="205"/>
+      <c r="G280" s="205"/>
+      <c r="H280" s="205"/>
+      <c r="I280" s="205"/>
+      <c r="J280" s="205"/>
+      <c r="K280" s="206"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -32950,16 +32955,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="186" t="s">
+      <c r="D286" s="204" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="187"/>
-      <c r="F286" s="187"/>
-      <c r="G286" s="187"/>
-      <c r="H286" s="187"/>
-      <c r="I286" s="187"/>
-      <c r="J286" s="187"/>
-      <c r="K286" s="188"/>
+      <c r="E286" s="205"/>
+      <c r="F286" s="205"/>
+      <c r="G286" s="205"/>
+      <c r="H286" s="205"/>
+      <c r="I286" s="205"/>
+      <c r="J286" s="205"/>
+      <c r="K286" s="206"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -33147,16 +33152,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="186" t="s">
+      <c r="D296" s="204" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="187"/>
-      <c r="F296" s="187"/>
-      <c r="G296" s="187"/>
-      <c r="H296" s="187"/>
-      <c r="I296" s="187"/>
-      <c r="J296" s="187"/>
-      <c r="K296" s="188"/>
+      <c r="E296" s="205"/>
+      <c r="F296" s="205"/>
+      <c r="G296" s="205"/>
+      <c r="H296" s="205"/>
+      <c r="I296" s="205"/>
+      <c r="J296" s="205"/>
+      <c r="K296" s="206"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -33187,16 +33192,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="203" t="s">
+      <c r="D298" s="188" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="199"/>
-      <c r="F298" s="199"/>
-      <c r="G298" s="199"/>
-      <c r="H298" s="199"/>
-      <c r="I298" s="199"/>
-      <c r="J298" s="199"/>
-      <c r="K298" s="200"/>
+      <c r="E298" s="189"/>
+      <c r="F298" s="189"/>
+      <c r="G298" s="189"/>
+      <c r="H298" s="189"/>
+      <c r="I298" s="189"/>
+      <c r="J298" s="189"/>
+      <c r="K298" s="190"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -33208,14 +33213,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="209"/>
-      <c r="E299" s="193"/>
-      <c r="F299" s="193"/>
-      <c r="G299" s="193"/>
-      <c r="H299" s="193"/>
-      <c r="I299" s="193"/>
-      <c r="J299" s="193"/>
-      <c r="K299" s="210"/>
+      <c r="D299" s="191"/>
+      <c r="E299" s="192"/>
+      <c r="F299" s="192"/>
+      <c r="G299" s="192"/>
+      <c r="H299" s="192"/>
+      <c r="I299" s="192"/>
+      <c r="J299" s="192"/>
+      <c r="K299" s="193"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -33227,16 +33232,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="203" t="s">
+      <c r="D300" s="188" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="199"/>
-      <c r="F300" s="199"/>
-      <c r="G300" s="199"/>
-      <c r="H300" s="199"/>
-      <c r="I300" s="199"/>
-      <c r="J300" s="199"/>
-      <c r="K300" s="200"/>
+      <c r="E300" s="189"/>
+      <c r="F300" s="189"/>
+      <c r="G300" s="189"/>
+      <c r="H300" s="189"/>
+      <c r="I300" s="189"/>
+      <c r="J300" s="189"/>
+      <c r="K300" s="190"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -33248,14 +33253,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="209"/>
-      <c r="E301" s="193"/>
-      <c r="F301" s="193"/>
-      <c r="G301" s="193"/>
-      <c r="H301" s="193"/>
-      <c r="I301" s="193"/>
-      <c r="J301" s="193"/>
-      <c r="K301" s="210"/>
+      <c r="D301" s="191"/>
+      <c r="E301" s="192"/>
+      <c r="F301" s="192"/>
+      <c r="G301" s="192"/>
+      <c r="H301" s="192"/>
+      <c r="I301" s="192"/>
+      <c r="J301" s="192"/>
+      <c r="K301" s="193"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -33267,16 +33272,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="203" t="s">
+      <c r="D302" s="188" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="199"/>
-      <c r="F302" s="199"/>
-      <c r="G302" s="199"/>
-      <c r="H302" s="199"/>
-      <c r="I302" s="199"/>
-      <c r="J302" s="199"/>
-      <c r="K302" s="200"/>
+      <c r="E302" s="189"/>
+      <c r="F302" s="189"/>
+      <c r="G302" s="189"/>
+      <c r="H302" s="189"/>
+      <c r="I302" s="189"/>
+      <c r="J302" s="189"/>
+      <c r="K302" s="190"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -33288,14 +33293,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="209"/>
-      <c r="E303" s="193"/>
-      <c r="F303" s="193"/>
-      <c r="G303" s="193"/>
-      <c r="H303" s="193"/>
-      <c r="I303" s="193"/>
-      <c r="J303" s="193"/>
-      <c r="K303" s="210"/>
+      <c r="D303" s="191"/>
+      <c r="E303" s="192"/>
+      <c r="F303" s="192"/>
+      <c r="G303" s="192"/>
+      <c r="H303" s="192"/>
+      <c r="I303" s="192"/>
+      <c r="J303" s="192"/>
+      <c r="K303" s="193"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -33307,16 +33312,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="203" t="s">
+      <c r="D304" s="188" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="199"/>
-      <c r="F304" s="199"/>
-      <c r="G304" s="199"/>
-      <c r="H304" s="199"/>
-      <c r="I304" s="199"/>
-      <c r="J304" s="199"/>
-      <c r="K304" s="200"/>
+      <c r="E304" s="189"/>
+      <c r="F304" s="189"/>
+      <c r="G304" s="189"/>
+      <c r="H304" s="189"/>
+      <c r="I304" s="189"/>
+      <c r="J304" s="189"/>
+      <c r="K304" s="190"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="31">
@@ -33328,14 +33333,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="32"/>
-      <c r="D305" s="209"/>
-      <c r="E305" s="193"/>
-      <c r="F305" s="193"/>
-      <c r="G305" s="193"/>
-      <c r="H305" s="193"/>
-      <c r="I305" s="193"/>
-      <c r="J305" s="193"/>
-      <c r="K305" s="210"/>
+      <c r="D305" s="191"/>
+      <c r="E305" s="192"/>
+      <c r="F305" s="192"/>
+      <c r="G305" s="192"/>
+      <c r="H305" s="192"/>
+      <c r="I305" s="192"/>
+      <c r="J305" s="192"/>
+      <c r="K305" s="193"/>
       <c r="L305" s="56"/>
       <c r="M305" s="57"/>
       <c r="N305" s="57"/>
@@ -33350,16 +33355,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="38"/>
-      <c r="D306" s="203" t="s">
+      <c r="D306" s="188" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="199"/>
-      <c r="F306" s="199"/>
-      <c r="G306" s="199"/>
-      <c r="H306" s="199"/>
-      <c r="I306" s="199"/>
-      <c r="J306" s="199"/>
-      <c r="K306" s="200"/>
+      <c r="E306" s="189"/>
+      <c r="F306" s="189"/>
+      <c r="G306" s="189"/>
+      <c r="H306" s="189"/>
+      <c r="I306" s="189"/>
+      <c r="J306" s="189"/>
+      <c r="K306" s="190"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -33371,14 +33376,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="209"/>
-      <c r="E307" s="193"/>
-      <c r="F307" s="193"/>
-      <c r="G307" s="193"/>
-      <c r="H307" s="193"/>
-      <c r="I307" s="193"/>
-      <c r="J307" s="193"/>
-      <c r="K307" s="210"/>
+      <c r="D307" s="191"/>
+      <c r="E307" s="192"/>
+      <c r="F307" s="192"/>
+      <c r="G307" s="192"/>
+      <c r="H307" s="192"/>
+      <c r="I307" s="192"/>
+      <c r="J307" s="192"/>
+      <c r="K307" s="193"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -33390,16 +33395,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="203" t="s">
+      <c r="D308" s="188" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="199"/>
-      <c r="F308" s="199"/>
-      <c r="G308" s="199"/>
-      <c r="H308" s="199"/>
-      <c r="I308" s="199"/>
-      <c r="J308" s="199"/>
-      <c r="K308" s="200"/>
+      <c r="E308" s="189"/>
+      <c r="F308" s="189"/>
+      <c r="G308" s="189"/>
+      <c r="H308" s="189"/>
+      <c r="I308" s="189"/>
+      <c r="J308" s="189"/>
+      <c r="K308" s="190"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -33411,14 +33416,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="209"/>
-      <c r="E309" s="193"/>
-      <c r="F309" s="193"/>
-      <c r="G309" s="193"/>
-      <c r="H309" s="193"/>
-      <c r="I309" s="193"/>
-      <c r="J309" s="193"/>
-      <c r="K309" s="210"/>
+      <c r="D309" s="191"/>
+      <c r="E309" s="192"/>
+      <c r="F309" s="192"/>
+      <c r="G309" s="192"/>
+      <c r="H309" s="192"/>
+      <c r="I309" s="192"/>
+      <c r="J309" s="192"/>
+      <c r="K309" s="193"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -37298,12 +37303,29 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D208:K208"/>
+    <mergeCell ref="D210:K210"/>
+    <mergeCell ref="D214:K214"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D200:K200"/>
+    <mergeCell ref="D202:K202"/>
     <mergeCell ref="D280:K280"/>
     <mergeCell ref="D286:K286"/>
     <mergeCell ref="D296:K296"/>
@@ -37320,29 +37342,12 @@
     <mergeCell ref="D250:K250"/>
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
-    <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D210:K210"/>
-    <mergeCell ref="D214:K214"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D200:K200"/>
-    <mergeCell ref="D202:K202"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape"/>
@@ -37732,7 +37737,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CA480A7D-7842-4326-A491-9C5672303D17}">
   <dimension ref="B2:H107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+    <sheetView topLeftCell="B10" workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
@@ -37748,25 +37753,25 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="30">
-      <c r="B2" s="222" t="s">
+      <c r="B2" s="184" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="222" t="s">
+      <c r="C2" s="184" t="s">
         <v>527</v>
       </c>
-      <c r="D2" s="222" t="s">
+      <c r="D2" s="184" t="s">
         <v>528</v>
       </c>
-      <c r="E2" s="222" t="s">
+      <c r="E2" s="184" t="s">
         <v>529</v>
       </c>
-      <c r="F2" s="222" t="s">
+      <c r="F2" s="184" t="s">
         <v>571</v>
       </c>
-      <c r="G2" s="223" t="s">
+      <c r="G2" s="185" t="s">
         <v>703</v>
       </c>
-      <c r="H2" s="223" t="s">
+      <c r="H2" s="185" t="s">
         <v>702</v>
       </c>
     </row>
@@ -39632,10 +39637,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="18.75">
-      <c r="B2" s="221" t="s">
+      <c r="B2" s="223" t="s">
         <v>475</v>
       </c>
-      <c r="C2" s="221"/>
+      <c r="C2" s="223"/>
     </row>
     <row r="3" spans="2:10" ht="15.75" thickBot="1"/>
     <row r="4" spans="2:10">

</xml_diff>

<commit_message>
last alpha before new v2.0.0.0
Fix : autotracking of Kara's location, Hieroglyphs and Mystic Statues with RAM addresses
Add : autotracking of hieroglyphs' slots by getting Journal (not forced to give it anymore before placing)
</commit_message>
<xml_diff>
--- a/autotracking/Switches.xlsx
+++ b/autotracking/Switches.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Apokalysme\LaunchMyCraft\git_repository\iogr_emotracker_apokalysme\autotracking\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1E84D46-FE15-4F9E-AB77-9E7E47873E45}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60DE9AE5-D93E-42CF-9D6A-394AC7AF2E54}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1825" uniqueCount="720">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1401" uniqueCount="732">
   <si>
     <t>ID</t>
   </si>
@@ -2204,6 +2204,42 @@
   </si>
   <si>
     <t>Talking to Teacher</t>
+  </si>
+  <si>
+    <t>Hieroglyph slot 1</t>
+  </si>
+  <si>
+    <t>Hieroglyph slot 2</t>
+  </si>
+  <si>
+    <t>Hieroglyph slot 3</t>
+  </si>
+  <si>
+    <t>Hieroglyph slot 4</t>
+  </si>
+  <si>
+    <t>Hieroglyph slot 5</t>
+  </si>
+  <si>
+    <t>Hieroglyph slot 6</t>
+  </si>
+  <si>
+    <t>Mystic Statue 1 needed</t>
+  </si>
+  <si>
+    <t>Mystic Statue 6 needed</t>
+  </si>
+  <si>
+    <t>Mystic Statue 5 needed</t>
+  </si>
+  <si>
+    <t>Mystic Statue 3 needed</t>
+  </si>
+  <si>
+    <t>Mystic Statue 2 needed</t>
+  </si>
+  <si>
+    <t>Kara's location (01 = Ed's, 02 = Mine, 03 = Angel, 04 = Kress, 05 = Ankor Wat)</t>
   </si>
 </sst>
 </file>
@@ -2458,7 +2494,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="55">
+  <borders count="58">
     <border>
       <left/>
       <right/>
@@ -3126,6 +3162,43 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -3133,7 +3206,7 @@
     <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="224">
+  <cellXfs count="227">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -3682,13 +3755,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="10" xfId="3" applyBorder="1" applyAlignment="1">
@@ -3697,13 +3806,13 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="28" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="12" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="9" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
@@ -3721,28 +3830,16 @@
     <xf numFmtId="0" fontId="6" fillId="3" borderId="13" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="27" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="11" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="25" xfId="3" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="41" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="7" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="32" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="36" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3763,38 +3860,23 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="39" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="39" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="7" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="42" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="20" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="33" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="23" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="3" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="3" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="55" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="56" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="57" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -4237,8 +4319,8 @@
   <dimension ref="A1:P1237"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J9" sqref="J9"/>
+      <pane ySplit="1" topLeftCell="A74" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D90" sqref="D90:K90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15"/>
@@ -4312,16 +4394,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="188" t="s">
+      <c r="D2" s="205" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="189"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="189"/>
-      <c r="I2" s="189"/>
-      <c r="J2" s="189"/>
-      <c r="K2" s="190"/>
+      <c r="E2" s="201"/>
+      <c r="F2" s="201"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="201"/>
+      <c r="J2" s="201"/>
+      <c r="K2" s="202"/>
       <c r="M2" s="81" t="s">
         <v>7</v>
       </c>
@@ -4339,14 +4421,14 @@
         <f t="shared" ref="C3:C33" si="1">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="194"/>
-      <c r="E3" s="195"/>
-      <c r="F3" s="195"/>
-      <c r="G3" s="195"/>
-      <c r="H3" s="195"/>
-      <c r="I3" s="195"/>
-      <c r="J3" s="195"/>
-      <c r="K3" s="196"/>
+      <c r="D3" s="206"/>
+      <c r="E3" s="207"/>
+      <c r="F3" s="207"/>
+      <c r="G3" s="207"/>
+      <c r="H3" s="207"/>
+      <c r="I3" s="207"/>
+      <c r="J3" s="207"/>
+      <c r="K3" s="208"/>
       <c r="M3" s="81" t="s">
         <v>8</v>
       </c>
@@ -7357,14 +7439,16 @@
         <v>A58</v>
       </c>
       <c r="C90" s="13"/>
-      <c r="D90" s="47"/>
-      <c r="E90" s="12"/>
-      <c r="F90" s="12"/>
-      <c r="G90" s="21"/>
-      <c r="H90" s="48"/>
-      <c r="I90" s="12"/>
-      <c r="J90" s="12"/>
-      <c r="K90" s="21"/>
+      <c r="D90" s="224" t="s">
+        <v>720</v>
+      </c>
+      <c r="E90" s="225"/>
+      <c r="F90" s="225"/>
+      <c r="G90" s="225"/>
+      <c r="H90" s="225"/>
+      <c r="I90" s="225"/>
+      <c r="J90" s="225"/>
+      <c r="K90" s="226"/>
     </row>
     <row r="91" spans="1:15">
       <c r="A91" s="12">
@@ -7376,14 +7460,16 @@
         <v>A59</v>
       </c>
       <c r="C91" s="13"/>
-      <c r="D91" s="47"/>
-      <c r="E91" s="12"/>
-      <c r="F91" s="12"/>
-      <c r="G91" s="21"/>
-      <c r="H91" s="48"/>
-      <c r="I91" s="12"/>
-      <c r="J91" s="12"/>
-      <c r="K91" s="21"/>
+      <c r="D91" s="224" t="s">
+        <v>721</v>
+      </c>
+      <c r="E91" s="225"/>
+      <c r="F91" s="225"/>
+      <c r="G91" s="225"/>
+      <c r="H91" s="225"/>
+      <c r="I91" s="225"/>
+      <c r="J91" s="225"/>
+      <c r="K91" s="226"/>
     </row>
     <row r="92" spans="1:15">
       <c r="A92" s="12">
@@ -7395,14 +7481,16 @@
         <v>A5A</v>
       </c>
       <c r="C92" s="13"/>
-      <c r="D92" s="47"/>
-      <c r="E92" s="12"/>
-      <c r="F92" s="12"/>
-      <c r="G92" s="21"/>
-      <c r="H92" s="48"/>
-      <c r="I92" s="12"/>
-      <c r="J92" s="12"/>
-      <c r="K92" s="21"/>
+      <c r="D92" s="224" t="s">
+        <v>722</v>
+      </c>
+      <c r="E92" s="225"/>
+      <c r="F92" s="225"/>
+      <c r="G92" s="225"/>
+      <c r="H92" s="225"/>
+      <c r="I92" s="225"/>
+      <c r="J92" s="225"/>
+      <c r="K92" s="226"/>
     </row>
     <row r="93" spans="1:15">
       <c r="A93" s="12">
@@ -7414,14 +7502,16 @@
         <v>A5B</v>
       </c>
       <c r="C93" s="13"/>
-      <c r="D93" s="47"/>
-      <c r="E93" s="12"/>
-      <c r="F93" s="12"/>
-      <c r="G93" s="21"/>
-      <c r="H93" s="48"/>
-      <c r="I93" s="12"/>
-      <c r="J93" s="12"/>
-      <c r="K93" s="21"/>
+      <c r="D93" s="224" t="s">
+        <v>723</v>
+      </c>
+      <c r="E93" s="225"/>
+      <c r="F93" s="225"/>
+      <c r="G93" s="225"/>
+      <c r="H93" s="225"/>
+      <c r="I93" s="225"/>
+      <c r="J93" s="225"/>
+      <c r="K93" s="226"/>
     </row>
     <row r="94" spans="1:15">
       <c r="A94" s="12">
@@ -7433,14 +7523,16 @@
         <v>A5C</v>
       </c>
       <c r="C94" s="13"/>
-      <c r="D94" s="47"/>
-      <c r="E94" s="12"/>
-      <c r="F94" s="12"/>
-      <c r="G94" s="21"/>
-      <c r="H94" s="48"/>
-      <c r="I94" s="12"/>
-      <c r="J94" s="12"/>
-      <c r="K94" s="21"/>
+      <c r="D94" s="224" t="s">
+        <v>724</v>
+      </c>
+      <c r="E94" s="225"/>
+      <c r="F94" s="225"/>
+      <c r="G94" s="225"/>
+      <c r="H94" s="225"/>
+      <c r="I94" s="225"/>
+      <c r="J94" s="225"/>
+      <c r="K94" s="226"/>
     </row>
     <row r="95" spans="1:15">
       <c r="A95" s="12">
@@ -7452,14 +7544,16 @@
         <v>A5D</v>
       </c>
       <c r="C95" s="13"/>
-      <c r="D95" s="47"/>
-      <c r="E95" s="12"/>
-      <c r="F95" s="12"/>
-      <c r="G95" s="21"/>
-      <c r="H95" s="48"/>
-      <c r="I95" s="12"/>
-      <c r="J95" s="12"/>
-      <c r="K95" s="21"/>
+      <c r="D95" s="224" t="s">
+        <v>725</v>
+      </c>
+      <c r="E95" s="225"/>
+      <c r="F95" s="225"/>
+      <c r="G95" s="225"/>
+      <c r="H95" s="225"/>
+      <c r="I95" s="225"/>
+      <c r="J95" s="225"/>
+      <c r="K95" s="226"/>
     </row>
     <row r="96" spans="1:15">
       <c r="A96" s="12">
@@ -7471,14 +7565,16 @@
         <v>A5E</v>
       </c>
       <c r="C96" s="13"/>
-      <c r="D96" s="47"/>
-      <c r="E96" s="12"/>
-      <c r="F96" s="12"/>
-      <c r="G96" s="21"/>
-      <c r="H96" s="48"/>
-      <c r="I96" s="12"/>
-      <c r="J96" s="12"/>
-      <c r="K96" s="21"/>
+      <c r="D96" s="224" t="s">
+        <v>731</v>
+      </c>
+      <c r="E96" s="225"/>
+      <c r="F96" s="225"/>
+      <c r="G96" s="225"/>
+      <c r="H96" s="225"/>
+      <c r="I96" s="225"/>
+      <c r="J96" s="225"/>
+      <c r="K96" s="226"/>
     </row>
     <row r="97" spans="1:15" s="1" customFormat="1">
       <c r="A97" s="31">
@@ -7492,12 +7588,24 @@
       <c r="C97" s="32"/>
       <c r="D97" s="49"/>
       <c r="E97" s="31"/>
-      <c r="F97" s="31"/>
-      <c r="G97" s="50"/>
-      <c r="H97" s="51"/>
-      <c r="I97" s="31"/>
-      <c r="J97" s="31"/>
-      <c r="K97" s="50"/>
+      <c r="F97" s="169" t="s">
+        <v>727</v>
+      </c>
+      <c r="G97" s="169" t="s">
+        <v>728</v>
+      </c>
+      <c r="H97" s="169" t="s">
+        <v>729</v>
+      </c>
+      <c r="I97" s="169" t="s">
+        <v>729</v>
+      </c>
+      <c r="J97" s="169" t="s">
+        <v>730</v>
+      </c>
+      <c r="K97" s="169" t="s">
+        <v>726</v>
+      </c>
       <c r="M97" s="56"/>
       <c r="N97" s="57"/>
       <c r="O97" s="57"/>
@@ -10405,16 +10513,16 @@
         <v>AA6</v>
       </c>
       <c r="C168" s="13"/>
-      <c r="D168" s="221" t="s">
+      <c r="D168" s="186" t="s">
         <v>348</v>
       </c>
-      <c r="E168" s="221"/>
-      <c r="F168" s="221"/>
-      <c r="G168" s="221"/>
-      <c r="H168" s="221"/>
-      <c r="I168" s="221"/>
-      <c r="J168" s="221"/>
-      <c r="K168" s="221"/>
+      <c r="E168" s="186"/>
+      <c r="F168" s="186"/>
+      <c r="G168" s="186"/>
+      <c r="H168" s="186"/>
+      <c r="I168" s="186"/>
+      <c r="J168" s="186"/>
+      <c r="K168" s="186"/>
     </row>
     <row r="169" spans="1:15">
       <c r="A169" s="12">
@@ -10540,16 +10648,16 @@
         <v>AAD</v>
       </c>
       <c r="C175" s="13"/>
-      <c r="D175" s="221" t="s">
+      <c r="D175" s="186" t="s">
         <v>349</v>
       </c>
-      <c r="E175" s="221"/>
-      <c r="F175" s="221"/>
-      <c r="G175" s="221"/>
-      <c r="H175" s="221"/>
-      <c r="I175" s="221"/>
-      <c r="J175" s="221"/>
-      <c r="K175" s="221"/>
+      <c r="E175" s="186"/>
+      <c r="F175" s="186"/>
+      <c r="G175" s="186"/>
+      <c r="H175" s="186"/>
+      <c r="I175" s="186"/>
+      <c r="J175" s="186"/>
+      <c r="K175" s="186"/>
     </row>
     <row r="176" spans="1:15">
       <c r="A176" s="12">
@@ -10602,16 +10710,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="38"/>
-      <c r="D178" s="222" t="s">
+      <c r="D178" s="187" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="221"/>
-      <c r="F178" s="221"/>
-      <c r="G178" s="221"/>
-      <c r="H178" s="221"/>
-      <c r="I178" s="221"/>
-      <c r="J178" s="221"/>
-      <c r="K178" s="221"/>
+      <c r="E178" s="186"/>
+      <c r="F178" s="186"/>
+      <c r="G178" s="186"/>
+      <c r="H178" s="186"/>
+      <c r="I178" s="186"/>
+      <c r="J178" s="186"/>
+      <c r="K178" s="186"/>
       <c r="L178" t="s">
         <v>424</v>
       </c>
@@ -10683,16 +10791,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="204" t="s">
+      <c r="D182" s="188" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="205"/>
-      <c r="F182" s="205"/>
-      <c r="G182" s="205"/>
-      <c r="H182" s="205"/>
-      <c r="I182" s="205"/>
-      <c r="J182" s="205"/>
-      <c r="K182" s="206"/>
+      <c r="E182" s="189"/>
+      <c r="F182" s="189"/>
+      <c r="G182" s="189"/>
+      <c r="H182" s="189"/>
+      <c r="I182" s="189"/>
+      <c r="J182" s="189"/>
+      <c r="K182" s="190"/>
     </row>
     <row r="183" spans="1:15">
       <c r="A183" s="12">
@@ -10704,16 +10812,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="204" t="s">
+      <c r="D183" s="188" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="205"/>
-      <c r="F183" s="205"/>
-      <c r="G183" s="205"/>
-      <c r="H183" s="205"/>
-      <c r="I183" s="205"/>
-      <c r="J183" s="205"/>
-      <c r="K183" s="206"/>
+      <c r="E183" s="189"/>
+      <c r="F183" s="189"/>
+      <c r="G183" s="189"/>
+      <c r="H183" s="189"/>
+      <c r="I183" s="189"/>
+      <c r="J183" s="189"/>
+      <c r="K183" s="190"/>
     </row>
     <row r="184" spans="1:15">
       <c r="A184" s="12">
@@ -10725,16 +10833,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="204" t="s">
+      <c r="D184" s="188" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="205"/>
-      <c r="F184" s="205"/>
-      <c r="G184" s="205"/>
-      <c r="H184" s="205"/>
-      <c r="I184" s="205"/>
-      <c r="J184" s="205"/>
-      <c r="K184" s="206"/>
+      <c r="E184" s="189"/>
+      <c r="F184" s="189"/>
+      <c r="G184" s="189"/>
+      <c r="H184" s="189"/>
+      <c r="I184" s="189"/>
+      <c r="J184" s="189"/>
+      <c r="K184" s="190"/>
     </row>
     <row r="185" spans="1:15">
       <c r="A185" s="12">
@@ -10746,16 +10854,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="204" t="s">
+      <c r="D185" s="188" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="205"/>
-      <c r="F185" s="205"/>
-      <c r="G185" s="205"/>
-      <c r="H185" s="205"/>
-      <c r="I185" s="205"/>
-      <c r="J185" s="205"/>
-      <c r="K185" s="206"/>
+      <c r="E185" s="189"/>
+      <c r="F185" s="189"/>
+      <c r="G185" s="189"/>
+      <c r="H185" s="189"/>
+      <c r="I185" s="189"/>
+      <c r="J185" s="189"/>
+      <c r="K185" s="190"/>
     </row>
     <row r="186" spans="1:15">
       <c r="A186" s="12">
@@ -10767,16 +10875,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="204" t="s">
+      <c r="D186" s="188" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="205"/>
-      <c r="F186" s="205"/>
-      <c r="G186" s="205"/>
-      <c r="H186" s="205"/>
-      <c r="I186" s="205"/>
-      <c r="J186" s="205"/>
-      <c r="K186" s="206"/>
+      <c r="E186" s="189"/>
+      <c r="F186" s="189"/>
+      <c r="G186" s="189"/>
+      <c r="H186" s="189"/>
+      <c r="I186" s="189"/>
+      <c r="J186" s="189"/>
+      <c r="K186" s="190"/>
     </row>
     <row r="187" spans="1:15">
       <c r="A187" s="12">
@@ -10788,16 +10896,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="204" t="s">
+      <c r="D187" s="188" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="205"/>
-      <c r="F187" s="205"/>
-      <c r="G187" s="205"/>
-      <c r="H187" s="205"/>
-      <c r="I187" s="205"/>
-      <c r="J187" s="205"/>
-      <c r="K187" s="206"/>
+      <c r="E187" s="189"/>
+      <c r="F187" s="189"/>
+      <c r="G187" s="189"/>
+      <c r="H187" s="189"/>
+      <c r="I187" s="189"/>
+      <c r="J187" s="189"/>
+      <c r="K187" s="190"/>
     </row>
     <row r="188" spans="1:15">
       <c r="A188" s="12">
@@ -10809,16 +10917,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="204" t="s">
+      <c r="D188" s="188" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="205"/>
-      <c r="F188" s="205"/>
-      <c r="G188" s="205"/>
-      <c r="H188" s="205"/>
-      <c r="I188" s="205"/>
-      <c r="J188" s="205"/>
-      <c r="K188" s="206"/>
+      <c r="E188" s="189"/>
+      <c r="F188" s="189"/>
+      <c r="G188" s="189"/>
+      <c r="H188" s="189"/>
+      <c r="I188" s="189"/>
+      <c r="J188" s="189"/>
+      <c r="K188" s="190"/>
     </row>
     <row r="189" spans="1:15">
       <c r="A189" s="12">
@@ -10830,16 +10938,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="204" t="s">
+      <c r="D189" s="188" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="205"/>
-      <c r="F189" s="205"/>
-      <c r="G189" s="205"/>
-      <c r="H189" s="205"/>
-      <c r="I189" s="205"/>
-      <c r="J189" s="205"/>
-      <c r="K189" s="206"/>
+      <c r="E189" s="189"/>
+      <c r="F189" s="189"/>
+      <c r="G189" s="189"/>
+      <c r="H189" s="189"/>
+      <c r="I189" s="189"/>
+      <c r="J189" s="189"/>
+      <c r="K189" s="190"/>
     </row>
     <row r="190" spans="1:15">
       <c r="A190" s="12">
@@ -10851,16 +10959,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="204" t="s">
+      <c r="D190" s="188" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="205"/>
-      <c r="F190" s="205"/>
-      <c r="G190" s="205"/>
-      <c r="H190" s="205"/>
-      <c r="I190" s="205"/>
-      <c r="J190" s="205"/>
-      <c r="K190" s="206"/>
+      <c r="E190" s="189"/>
+      <c r="F190" s="189"/>
+      <c r="G190" s="189"/>
+      <c r="H190" s="189"/>
+      <c r="I190" s="189"/>
+      <c r="J190" s="189"/>
+      <c r="K190" s="190"/>
     </row>
     <row r="191" spans="1:15">
       <c r="A191" s="12">
@@ -10872,16 +10980,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="204" t="s">
+      <c r="D191" s="188" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="205"/>
-      <c r="F191" s="205"/>
-      <c r="G191" s="205"/>
-      <c r="H191" s="205"/>
-      <c r="I191" s="205"/>
-      <c r="J191" s="205"/>
-      <c r="K191" s="206"/>
+      <c r="E191" s="189"/>
+      <c r="F191" s="189"/>
+      <c r="G191" s="189"/>
+      <c r="H191" s="189"/>
+      <c r="I191" s="189"/>
+      <c r="J191" s="189"/>
+      <c r="K191" s="190"/>
     </row>
     <row r="192" spans="1:15">
       <c r="A192" s="12">
@@ -10893,16 +11001,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="204" t="s">
+      <c r="D192" s="188" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="205"/>
-      <c r="F192" s="205"/>
-      <c r="G192" s="205"/>
-      <c r="H192" s="205"/>
-      <c r="I192" s="205"/>
-      <c r="J192" s="205"/>
-      <c r="K192" s="206"/>
+      <c r="E192" s="189"/>
+      <c r="F192" s="189"/>
+      <c r="G192" s="189"/>
+      <c r="H192" s="189"/>
+      <c r="I192" s="189"/>
+      <c r="J192" s="189"/>
+      <c r="K192" s="190"/>
     </row>
     <row r="193" spans="1:15" s="1" customFormat="1">
       <c r="A193" s="31">
@@ -10914,16 +11022,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="32"/>
-      <c r="D193" s="218" t="s">
+      <c r="D193" s="191" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="219"/>
-      <c r="F193" s="219"/>
-      <c r="G193" s="219"/>
-      <c r="H193" s="219"/>
-      <c r="I193" s="219"/>
-      <c r="J193" s="219"/>
-      <c r="K193" s="220"/>
+      <c r="E193" s="192"/>
+      <c r="F193" s="192"/>
+      <c r="G193" s="192"/>
+      <c r="H193" s="192"/>
+      <c r="I193" s="192"/>
+      <c r="J193" s="192"/>
+      <c r="K193" s="193"/>
       <c r="M193" s="56"/>
       <c r="N193" s="57"/>
       <c r="O193" s="57"/>
@@ -10938,16 +11046,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="38"/>
-      <c r="D194" s="199" t="s">
+      <c r="D194" s="194" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="192"/>
-      <c r="F194" s="192"/>
-      <c r="G194" s="192"/>
-      <c r="H194" s="192"/>
-      <c r="I194" s="192"/>
-      <c r="J194" s="192"/>
-      <c r="K194" s="200"/>
+      <c r="E194" s="195"/>
+      <c r="F194" s="195"/>
+      <c r="G194" s="195"/>
+      <c r="H194" s="195"/>
+      <c r="I194" s="195"/>
+      <c r="J194" s="195"/>
+      <c r="K194" s="196"/>
     </row>
     <row r="195" spans="1:15">
       <c r="A195" s="12">
@@ -10959,16 +11067,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="204" t="s">
+      <c r="D195" s="188" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="205"/>
-      <c r="F195" s="205"/>
-      <c r="G195" s="205"/>
-      <c r="H195" s="205"/>
-      <c r="I195" s="205"/>
-      <c r="J195" s="205"/>
-      <c r="K195" s="206"/>
+      <c r="E195" s="189"/>
+      <c r="F195" s="189"/>
+      <c r="G195" s="189"/>
+      <c r="H195" s="189"/>
+      <c r="I195" s="189"/>
+      <c r="J195" s="189"/>
+      <c r="K195" s="190"/>
     </row>
     <row r="196" spans="1:15">
       <c r="A196" s="12">
@@ -10980,16 +11088,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="204" t="s">
+      <c r="D196" s="188" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="205"/>
-      <c r="F196" s="205"/>
-      <c r="G196" s="205"/>
-      <c r="H196" s="205"/>
-      <c r="I196" s="205"/>
-      <c r="J196" s="205"/>
-      <c r="K196" s="206"/>
+      <c r="E196" s="189"/>
+      <c r="F196" s="189"/>
+      <c r="G196" s="189"/>
+      <c r="H196" s="189"/>
+      <c r="I196" s="189"/>
+      <c r="J196" s="189"/>
+      <c r="K196" s="190"/>
     </row>
     <row r="197" spans="1:15">
       <c r="A197" s="12">
@@ -11001,16 +11109,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="204" t="s">
+      <c r="D197" s="188" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="205"/>
-      <c r="F197" s="205"/>
-      <c r="G197" s="205"/>
-      <c r="H197" s="205"/>
-      <c r="I197" s="205"/>
-      <c r="J197" s="205"/>
-      <c r="K197" s="206"/>
+      <c r="E197" s="189"/>
+      <c r="F197" s="189"/>
+      <c r="G197" s="189"/>
+      <c r="H197" s="189"/>
+      <c r="I197" s="189"/>
+      <c r="J197" s="189"/>
+      <c r="K197" s="190"/>
     </row>
     <row r="198" spans="1:15">
       <c r="A198" s="12">
@@ -11022,16 +11130,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="204" t="s">
+      <c r="D198" s="188" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="205"/>
-      <c r="F198" s="205"/>
-      <c r="G198" s="205"/>
-      <c r="H198" s="205"/>
-      <c r="I198" s="205"/>
-      <c r="J198" s="205"/>
-      <c r="K198" s="206"/>
+      <c r="E198" s="189"/>
+      <c r="F198" s="189"/>
+      <c r="G198" s="189"/>
+      <c r="H198" s="189"/>
+      <c r="I198" s="189"/>
+      <c r="J198" s="189"/>
+      <c r="K198" s="190"/>
     </row>
     <row r="199" spans="1:15">
       <c r="A199" s="12">
@@ -11062,16 +11170,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="204" t="s">
+      <c r="D200" s="188" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="205"/>
-      <c r="F200" s="205"/>
-      <c r="G200" s="205"/>
-      <c r="H200" s="205"/>
-      <c r="I200" s="205"/>
-      <c r="J200" s="205"/>
-      <c r="K200" s="206"/>
+      <c r="E200" s="189"/>
+      <c r="F200" s="189"/>
+      <c r="G200" s="189"/>
+      <c r="H200" s="189"/>
+      <c r="I200" s="189"/>
+      <c r="J200" s="189"/>
+      <c r="K200" s="190"/>
     </row>
     <row r="201" spans="1:15">
       <c r="A201" s="12">
@@ -11102,16 +11210,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="210" t="s">
+      <c r="D202" s="218" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="211"/>
-      <c r="F202" s="211"/>
-      <c r="G202" s="211"/>
-      <c r="H202" s="211"/>
-      <c r="I202" s="211"/>
-      <c r="J202" s="211"/>
-      <c r="K202" s="212"/>
+      <c r="E202" s="219"/>
+      <c r="F202" s="219"/>
+      <c r="G202" s="219"/>
+      <c r="H202" s="219"/>
+      <c r="I202" s="219"/>
+      <c r="J202" s="219"/>
+      <c r="K202" s="220"/>
     </row>
     <row r="203" spans="1:15">
       <c r="A203" s="12">
@@ -11142,16 +11250,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="204" t="s">
+      <c r="D204" s="188" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="205"/>
-      <c r="F204" s="205"/>
-      <c r="G204" s="205"/>
-      <c r="H204" s="205"/>
-      <c r="I204" s="205"/>
-      <c r="J204" s="205"/>
-      <c r="K204" s="206"/>
+      <c r="E204" s="189"/>
+      <c r="F204" s="189"/>
+      <c r="G204" s="189"/>
+      <c r="H204" s="189"/>
+      <c r="I204" s="189"/>
+      <c r="J204" s="189"/>
+      <c r="K204" s="190"/>
     </row>
     <row r="205" spans="1:15">
       <c r="A205" s="12">
@@ -11182,16 +11290,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="204" t="s">
+      <c r="D206" s="188" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="205"/>
-      <c r="F206" s="205"/>
-      <c r="G206" s="205"/>
-      <c r="H206" s="205"/>
-      <c r="I206" s="205"/>
-      <c r="J206" s="205"/>
-      <c r="K206" s="206"/>
+      <c r="E206" s="189"/>
+      <c r="F206" s="189"/>
+      <c r="G206" s="189"/>
+      <c r="H206" s="189"/>
+      <c r="I206" s="189"/>
+      <c r="J206" s="189"/>
+      <c r="K206" s="190"/>
     </row>
     <row r="207" spans="1:15">
       <c r="A207" s="12">
@@ -11222,16 +11330,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="204" t="s">
+      <c r="D208" s="188" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="205"/>
-      <c r="F208" s="205"/>
-      <c r="G208" s="205"/>
-      <c r="H208" s="205"/>
-      <c r="I208" s="205"/>
-      <c r="J208" s="205"/>
-      <c r="K208" s="206"/>
+      <c r="E208" s="189"/>
+      <c r="F208" s="189"/>
+      <c r="G208" s="189"/>
+      <c r="H208" s="189"/>
+      <c r="I208" s="189"/>
+      <c r="J208" s="189"/>
+      <c r="K208" s="190"/>
     </row>
     <row r="209" spans="1:15" s="1" customFormat="1">
       <c r="A209" s="31">
@@ -11265,16 +11373,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="38"/>
-      <c r="D210" s="199" t="s">
+      <c r="D210" s="194" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="192"/>
-      <c r="F210" s="192"/>
-      <c r="G210" s="192"/>
-      <c r="H210" s="192"/>
-      <c r="I210" s="192"/>
-      <c r="J210" s="192"/>
-      <c r="K210" s="200"/>
+      <c r="E210" s="195"/>
+      <c r="F210" s="195"/>
+      <c r="G210" s="195"/>
+      <c r="H210" s="195"/>
+      <c r="I210" s="195"/>
+      <c r="J210" s="195"/>
+      <c r="K210" s="196"/>
     </row>
     <row r="211" spans="1:15">
       <c r="A211" s="12">
@@ -11343,16 +11451,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="204" t="s">
+      <c r="D214" s="188" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="205"/>
-      <c r="F214" s="205"/>
-      <c r="G214" s="205"/>
-      <c r="H214" s="205"/>
-      <c r="I214" s="205"/>
-      <c r="J214" s="205"/>
-      <c r="K214" s="206"/>
+      <c r="E214" s="189"/>
+      <c r="F214" s="189"/>
+      <c r="G214" s="189"/>
+      <c r="H214" s="189"/>
+      <c r="I214" s="189"/>
+      <c r="J214" s="189"/>
+      <c r="K214" s="190"/>
     </row>
     <row r="215" spans="1:15">
       <c r="A215" s="12">
@@ -11383,16 +11491,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="197" t="s">
+      <c r="D216" s="209" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="189"/>
-      <c r="F216" s="189"/>
-      <c r="G216" s="189"/>
-      <c r="H216" s="189"/>
-      <c r="I216" s="189"/>
-      <c r="J216" s="189"/>
-      <c r="K216" s="198"/>
+      <c r="E216" s="201"/>
+      <c r="F216" s="201"/>
+      <c r="G216" s="201"/>
+      <c r="H216" s="201"/>
+      <c r="I216" s="201"/>
+      <c r="J216" s="201"/>
+      <c r="K216" s="210"/>
     </row>
     <row r="217" spans="1:15">
       <c r="A217" s="12">
@@ -11404,14 +11512,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="199"/>
-      <c r="E217" s="192"/>
-      <c r="F217" s="192"/>
-      <c r="G217" s="192"/>
-      <c r="H217" s="192"/>
-      <c r="I217" s="192"/>
-      <c r="J217" s="192"/>
-      <c r="K217" s="200"/>
+      <c r="D217" s="194"/>
+      <c r="E217" s="195"/>
+      <c r="F217" s="195"/>
+      <c r="G217" s="195"/>
+      <c r="H217" s="195"/>
+      <c r="I217" s="195"/>
+      <c r="J217" s="195"/>
+      <c r="K217" s="196"/>
     </row>
     <row r="218" spans="1:15">
       <c r="A218" s="12">
@@ -11423,16 +11531,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="197" t="s">
+      <c r="D218" s="209" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="189"/>
-      <c r="F218" s="189"/>
-      <c r="G218" s="189"/>
-      <c r="H218" s="189"/>
-      <c r="I218" s="189"/>
-      <c r="J218" s="189"/>
-      <c r="K218" s="198"/>
+      <c r="E218" s="201"/>
+      <c r="F218" s="201"/>
+      <c r="G218" s="201"/>
+      <c r="H218" s="201"/>
+      <c r="I218" s="201"/>
+      <c r="J218" s="201"/>
+      <c r="K218" s="210"/>
     </row>
     <row r="219" spans="1:15">
       <c r="A219" s="12">
@@ -11444,14 +11552,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="199"/>
-      <c r="E219" s="192"/>
-      <c r="F219" s="192"/>
-      <c r="G219" s="192"/>
-      <c r="H219" s="192"/>
-      <c r="I219" s="192"/>
-      <c r="J219" s="192"/>
-      <c r="K219" s="200"/>
+      <c r="D219" s="194"/>
+      <c r="E219" s="195"/>
+      <c r="F219" s="195"/>
+      <c r="G219" s="195"/>
+      <c r="H219" s="195"/>
+      <c r="I219" s="195"/>
+      <c r="J219" s="195"/>
+      <c r="K219" s="196"/>
     </row>
     <row r="220" spans="1:15">
       <c r="A220" s="12">
@@ -11463,16 +11571,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="197" t="s">
+      <c r="D220" s="209" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="189"/>
-      <c r="F220" s="189"/>
-      <c r="G220" s="189"/>
-      <c r="H220" s="189"/>
-      <c r="I220" s="189"/>
-      <c r="J220" s="189"/>
-      <c r="K220" s="198"/>
+      <c r="E220" s="201"/>
+      <c r="F220" s="201"/>
+      <c r="G220" s="201"/>
+      <c r="H220" s="201"/>
+      <c r="I220" s="201"/>
+      <c r="J220" s="201"/>
+      <c r="K220" s="210"/>
     </row>
     <row r="221" spans="1:15">
       <c r="A221" s="12">
@@ -11484,14 +11592,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="199"/>
-      <c r="E221" s="192"/>
-      <c r="F221" s="192"/>
-      <c r="G221" s="192"/>
-      <c r="H221" s="192"/>
-      <c r="I221" s="192"/>
-      <c r="J221" s="192"/>
-      <c r="K221" s="200"/>
+      <c r="D221" s="194"/>
+      <c r="E221" s="195"/>
+      <c r="F221" s="195"/>
+      <c r="G221" s="195"/>
+      <c r="H221" s="195"/>
+      <c r="I221" s="195"/>
+      <c r="J221" s="195"/>
+      <c r="K221" s="196"/>
     </row>
     <row r="222" spans="1:15">
       <c r="A222" s="12">
@@ -11503,16 +11611,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="204" t="s">
+      <c r="D222" s="188" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="205"/>
-      <c r="F222" s="205"/>
-      <c r="G222" s="205"/>
-      <c r="H222" s="205"/>
-      <c r="I222" s="205"/>
-      <c r="J222" s="205"/>
-      <c r="K222" s="206"/>
+      <c r="E222" s="189"/>
+      <c r="F222" s="189"/>
+      <c r="G222" s="189"/>
+      <c r="H222" s="189"/>
+      <c r="I222" s="189"/>
+      <c r="J222" s="189"/>
+      <c r="K222" s="190"/>
     </row>
     <row r="223" spans="1:15">
       <c r="A223" s="12">
@@ -11543,16 +11651,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="204" t="s">
+      <c r="D224" s="188" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="205"/>
-      <c r="F224" s="205"/>
-      <c r="G224" s="205"/>
-      <c r="H224" s="205"/>
-      <c r="I224" s="205"/>
-      <c r="J224" s="205"/>
-      <c r="K224" s="206"/>
+      <c r="E224" s="189"/>
+      <c r="F224" s="189"/>
+      <c r="G224" s="189"/>
+      <c r="H224" s="189"/>
+      <c r="I224" s="189"/>
+      <c r="J224" s="189"/>
+      <c r="K224" s="190"/>
     </row>
     <row r="225" spans="1:15" s="1" customFormat="1">
       <c r="A225" s="31">
@@ -11586,16 +11694,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="38"/>
-      <c r="D226" s="207" t="s">
+      <c r="D226" s="215" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="208"/>
-      <c r="F226" s="208"/>
-      <c r="G226" s="208"/>
-      <c r="H226" s="208"/>
-      <c r="I226" s="208"/>
-      <c r="J226" s="208"/>
-      <c r="K226" s="209"/>
+      <c r="E226" s="216"/>
+      <c r="F226" s="216"/>
+      <c r="G226" s="216"/>
+      <c r="H226" s="216"/>
+      <c r="I226" s="216"/>
+      <c r="J226" s="216"/>
+      <c r="K226" s="217"/>
     </row>
     <row r="227" spans="1:15">
       <c r="A227" s="12">
@@ -11740,16 +11848,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="201" t="s">
+      <c r="D234" s="213" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="202"/>
-      <c r="F234" s="202"/>
-      <c r="G234" s="202"/>
-      <c r="H234" s="202"/>
-      <c r="I234" s="202"/>
-      <c r="J234" s="202"/>
-      <c r="K234" s="203"/>
+      <c r="E234" s="198"/>
+      <c r="F234" s="198"/>
+      <c r="G234" s="198"/>
+      <c r="H234" s="198"/>
+      <c r="I234" s="198"/>
+      <c r="J234" s="198"/>
+      <c r="K234" s="214"/>
     </row>
     <row r="235" spans="1:15">
       <c r="A235" s="12">
@@ -11818,16 +11926,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="188" t="s">
+      <c r="D238" s="205" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="189"/>
-      <c r="F238" s="189"/>
-      <c r="G238" s="189"/>
-      <c r="H238" s="189"/>
-      <c r="I238" s="189"/>
-      <c r="J238" s="189"/>
-      <c r="K238" s="190"/>
+      <c r="E238" s="201"/>
+      <c r="F238" s="201"/>
+      <c r="G238" s="201"/>
+      <c r="H238" s="201"/>
+      <c r="I238" s="201"/>
+      <c r="J238" s="201"/>
+      <c r="K238" s="202"/>
     </row>
     <row r="239" spans="1:15">
       <c r="A239" s="12">
@@ -11839,14 +11947,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="191"/>
-      <c r="E239" s="192"/>
-      <c r="F239" s="192"/>
-      <c r="G239" s="192"/>
-      <c r="H239" s="192"/>
-      <c r="I239" s="192"/>
-      <c r="J239" s="192"/>
-      <c r="K239" s="193"/>
+      <c r="D239" s="211"/>
+      <c r="E239" s="195"/>
+      <c r="F239" s="195"/>
+      <c r="G239" s="195"/>
+      <c r="H239" s="195"/>
+      <c r="I239" s="195"/>
+      <c r="J239" s="195"/>
+      <c r="K239" s="212"/>
     </row>
     <row r="240" spans="1:15">
       <c r="A240" s="12">
@@ -11858,16 +11966,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="68"/>
-      <c r="D240" s="189" t="s">
+      <c r="D240" s="201" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="189"/>
-      <c r="F240" s="189"/>
-      <c r="G240" s="189"/>
-      <c r="H240" s="189"/>
-      <c r="I240" s="189"/>
-      <c r="J240" s="189"/>
-      <c r="K240" s="190"/>
+      <c r="E240" s="201"/>
+      <c r="F240" s="201"/>
+      <c r="G240" s="201"/>
+      <c r="H240" s="201"/>
+      <c r="I240" s="201"/>
+      <c r="J240" s="201"/>
+      <c r="K240" s="202"/>
     </row>
     <row r="241" spans="1:15" s="1" customFormat="1">
       <c r="A241" s="31">
@@ -11879,14 +11987,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="33"/>
-      <c r="D241" s="216"/>
-      <c r="E241" s="216"/>
-      <c r="F241" s="216"/>
-      <c r="G241" s="216"/>
-      <c r="H241" s="216"/>
-      <c r="I241" s="216"/>
-      <c r="J241" s="216"/>
-      <c r="K241" s="217"/>
+      <c r="D241" s="203"/>
+      <c r="E241" s="203"/>
+      <c r="F241" s="203"/>
+      <c r="G241" s="203"/>
+      <c r="H241" s="203"/>
+      <c r="I241" s="203"/>
+      <c r="J241" s="203"/>
+      <c r="K241" s="204"/>
       <c r="M241" s="56"/>
       <c r="N241" s="57"/>
       <c r="O241" s="57"/>
@@ -12077,16 +12185,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="213" t="s">
+      <c r="D250" s="197" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="202"/>
-      <c r="F250" s="202"/>
-      <c r="G250" s="202"/>
-      <c r="H250" s="202"/>
-      <c r="I250" s="202"/>
-      <c r="J250" s="202"/>
-      <c r="K250" s="214"/>
+      <c r="E250" s="198"/>
+      <c r="F250" s="198"/>
+      <c r="G250" s="198"/>
+      <c r="H250" s="198"/>
+      <c r="I250" s="198"/>
+      <c r="J250" s="198"/>
+      <c r="K250" s="199"/>
     </row>
     <row r="251" spans="1:15">
       <c r="A251" s="12">
@@ -12655,16 +12763,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="215" t="s">
+      <c r="D280" s="200" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="205"/>
-      <c r="F280" s="205"/>
-      <c r="G280" s="205"/>
-      <c r="H280" s="205"/>
-      <c r="I280" s="205"/>
-      <c r="J280" s="205"/>
-      <c r="K280" s="206"/>
+      <c r="E280" s="189"/>
+      <c r="F280" s="189"/>
+      <c r="G280" s="189"/>
+      <c r="H280" s="189"/>
+      <c r="I280" s="189"/>
+      <c r="J280" s="189"/>
+      <c r="K280" s="190"/>
     </row>
     <row r="281" spans="1:15">
       <c r="A281" s="12">
@@ -12771,16 +12879,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="215" t="s">
+      <c r="D286" s="200" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="205"/>
-      <c r="F286" s="205"/>
-      <c r="G286" s="205"/>
-      <c r="H286" s="205"/>
-      <c r="I286" s="205"/>
-      <c r="J286" s="205"/>
-      <c r="K286" s="206"/>
+      <c r="E286" s="189"/>
+      <c r="F286" s="189"/>
+      <c r="G286" s="189"/>
+      <c r="H286" s="189"/>
+      <c r="I286" s="189"/>
+      <c r="J286" s="189"/>
+      <c r="K286" s="190"/>
     </row>
     <row r="287" spans="1:15">
       <c r="A287" s="12">
@@ -12968,16 +13076,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="204" t="s">
+      <c r="D296" s="188" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="205"/>
-      <c r="F296" s="205"/>
-      <c r="G296" s="205"/>
-      <c r="H296" s="205"/>
-      <c r="I296" s="205"/>
-      <c r="J296" s="205"/>
-      <c r="K296" s="206"/>
+      <c r="E296" s="189"/>
+      <c r="F296" s="189"/>
+      <c r="G296" s="189"/>
+      <c r="H296" s="189"/>
+      <c r="I296" s="189"/>
+      <c r="J296" s="189"/>
+      <c r="K296" s="190"/>
     </row>
     <row r="297" spans="1:15">
       <c r="A297" s="12">
@@ -13008,16 +13116,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="188" t="s">
+      <c r="D298" s="205" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="189"/>
-      <c r="F298" s="189"/>
-      <c r="G298" s="189"/>
-      <c r="H298" s="189"/>
-      <c r="I298" s="189"/>
-      <c r="J298" s="189"/>
-      <c r="K298" s="190"/>
+      <c r="E298" s="201"/>
+      <c r="F298" s="201"/>
+      <c r="G298" s="201"/>
+      <c r="H298" s="201"/>
+      <c r="I298" s="201"/>
+      <c r="J298" s="201"/>
+      <c r="K298" s="202"/>
     </row>
     <row r="299" spans="1:15">
       <c r="A299" s="12">
@@ -13029,14 +13137,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="191"/>
-      <c r="E299" s="192"/>
-      <c r="F299" s="192"/>
-      <c r="G299" s="192"/>
-      <c r="H299" s="192"/>
-      <c r="I299" s="192"/>
-      <c r="J299" s="192"/>
-      <c r="K299" s="193"/>
+      <c r="D299" s="211"/>
+      <c r="E299" s="195"/>
+      <c r="F299" s="195"/>
+      <c r="G299" s="195"/>
+      <c r="H299" s="195"/>
+      <c r="I299" s="195"/>
+      <c r="J299" s="195"/>
+      <c r="K299" s="212"/>
     </row>
     <row r="300" spans="1:15">
       <c r="A300" s="12">
@@ -13048,16 +13156,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="188" t="s">
+      <c r="D300" s="205" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="189"/>
-      <c r="F300" s="189"/>
-      <c r="G300" s="189"/>
-      <c r="H300" s="189"/>
-      <c r="I300" s="189"/>
-      <c r="J300" s="189"/>
-      <c r="K300" s="190"/>
+      <c r="E300" s="201"/>
+      <c r="F300" s="201"/>
+      <c r="G300" s="201"/>
+      <c r="H300" s="201"/>
+      <c r="I300" s="201"/>
+      <c r="J300" s="201"/>
+      <c r="K300" s="202"/>
     </row>
     <row r="301" spans="1:15">
       <c r="A301" s="12">
@@ -13069,14 +13177,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="191"/>
-      <c r="E301" s="192"/>
-      <c r="F301" s="192"/>
-      <c r="G301" s="192"/>
-      <c r="H301" s="192"/>
-      <c r="I301" s="192"/>
-      <c r="J301" s="192"/>
-      <c r="K301" s="193"/>
+      <c r="D301" s="211"/>
+      <c r="E301" s="195"/>
+      <c r="F301" s="195"/>
+      <c r="G301" s="195"/>
+      <c r="H301" s="195"/>
+      <c r="I301" s="195"/>
+      <c r="J301" s="195"/>
+      <c r="K301" s="212"/>
     </row>
     <row r="302" spans="1:15">
       <c r="A302" s="12">
@@ -13088,16 +13196,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="188" t="s">
+      <c r="D302" s="205" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="189"/>
-      <c r="F302" s="189"/>
-      <c r="G302" s="189"/>
-      <c r="H302" s="189"/>
-      <c r="I302" s="189"/>
-      <c r="J302" s="189"/>
-      <c r="K302" s="190"/>
+      <c r="E302" s="201"/>
+      <c r="F302" s="201"/>
+      <c r="G302" s="201"/>
+      <c r="H302" s="201"/>
+      <c r="I302" s="201"/>
+      <c r="J302" s="201"/>
+      <c r="K302" s="202"/>
     </row>
     <row r="303" spans="1:15">
       <c r="A303" s="12">
@@ -13109,14 +13217,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="191"/>
-      <c r="E303" s="192"/>
-      <c r="F303" s="192"/>
-      <c r="G303" s="192"/>
-      <c r="H303" s="192"/>
-      <c r="I303" s="192"/>
-      <c r="J303" s="192"/>
-      <c r="K303" s="193"/>
+      <c r="D303" s="211"/>
+      <c r="E303" s="195"/>
+      <c r="F303" s="195"/>
+      <c r="G303" s="195"/>
+      <c r="H303" s="195"/>
+      <c r="I303" s="195"/>
+      <c r="J303" s="195"/>
+      <c r="K303" s="212"/>
     </row>
     <row r="304" spans="1:15">
       <c r="A304" s="12">
@@ -13128,16 +13236,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="188" t="s">
+      <c r="D304" s="205" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="189"/>
-      <c r="F304" s="189"/>
-      <c r="G304" s="189"/>
-      <c r="H304" s="189"/>
-      <c r="I304" s="189"/>
-      <c r="J304" s="189"/>
-      <c r="K304" s="190"/>
+      <c r="E304" s="201"/>
+      <c r="F304" s="201"/>
+      <c r="G304" s="201"/>
+      <c r="H304" s="201"/>
+      <c r="I304" s="201"/>
+      <c r="J304" s="201"/>
+      <c r="K304" s="202"/>
     </row>
     <row r="305" spans="1:15" s="1" customFormat="1">
       <c r="A305" s="31">
@@ -13149,14 +13257,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="32"/>
-      <c r="D305" s="191"/>
-      <c r="E305" s="192"/>
-      <c r="F305" s="192"/>
-      <c r="G305" s="192"/>
-      <c r="H305" s="192"/>
-      <c r="I305" s="192"/>
-      <c r="J305" s="192"/>
-      <c r="K305" s="193"/>
+      <c r="D305" s="211"/>
+      <c r="E305" s="195"/>
+      <c r="F305" s="195"/>
+      <c r="G305" s="195"/>
+      <c r="H305" s="195"/>
+      <c r="I305" s="195"/>
+      <c r="J305" s="195"/>
+      <c r="K305" s="212"/>
       <c r="M305" s="56"/>
       <c r="N305" s="57"/>
       <c r="O305" s="57"/>
@@ -13171,16 +13279,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="38"/>
-      <c r="D306" s="188" t="s">
+      <c r="D306" s="205" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="189"/>
-      <c r="F306" s="189"/>
-      <c r="G306" s="189"/>
-      <c r="H306" s="189"/>
-      <c r="I306" s="189"/>
-      <c r="J306" s="189"/>
-      <c r="K306" s="190"/>
+      <c r="E306" s="201"/>
+      <c r="F306" s="201"/>
+      <c r="G306" s="201"/>
+      <c r="H306" s="201"/>
+      <c r="I306" s="201"/>
+      <c r="J306" s="201"/>
+      <c r="K306" s="202"/>
     </row>
     <row r="307" spans="1:15">
       <c r="A307" s="12">
@@ -13192,14 +13300,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="191"/>
-      <c r="E307" s="192"/>
-      <c r="F307" s="192"/>
-      <c r="G307" s="192"/>
-      <c r="H307" s="192"/>
-      <c r="I307" s="192"/>
-      <c r="J307" s="192"/>
-      <c r="K307" s="193"/>
+      <c r="D307" s="211"/>
+      <c r="E307" s="195"/>
+      <c r="F307" s="195"/>
+      <c r="G307" s="195"/>
+      <c r="H307" s="195"/>
+      <c r="I307" s="195"/>
+      <c r="J307" s="195"/>
+      <c r="K307" s="212"/>
     </row>
     <row r="308" spans="1:15">
       <c r="A308" s="12">
@@ -13211,16 +13319,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="188" t="s">
+      <c r="D308" s="205" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="189"/>
-      <c r="F308" s="189"/>
-      <c r="G308" s="189"/>
-      <c r="H308" s="189"/>
-      <c r="I308" s="189"/>
-      <c r="J308" s="189"/>
-      <c r="K308" s="190"/>
+      <c r="E308" s="201"/>
+      <c r="F308" s="201"/>
+      <c r="G308" s="201"/>
+      <c r="H308" s="201"/>
+      <c r="I308" s="201"/>
+      <c r="J308" s="201"/>
+      <c r="K308" s="202"/>
     </row>
     <row r="309" spans="1:15">
       <c r="A309" s="12">
@@ -13232,14 +13340,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="191"/>
-      <c r="E309" s="192"/>
-      <c r="F309" s="192"/>
-      <c r="G309" s="192"/>
-      <c r="H309" s="192"/>
-      <c r="I309" s="192"/>
-      <c r="J309" s="192"/>
-      <c r="K309" s="193"/>
+      <c r="D309" s="211"/>
+      <c r="E309" s="195"/>
+      <c r="F309" s="195"/>
+      <c r="G309" s="195"/>
+      <c r="H309" s="195"/>
+      <c r="I309" s="195"/>
+      <c r="J309" s="195"/>
+      <c r="K309" s="212"/>
     </row>
     <row r="310" spans="1:15">
       <c r="A310" s="12">
@@ -21526,16 +21634,16 @@
         <f t="shared" si="35"/>
         <v>DB8</v>
       </c>
-      <c r="D954" s="186" t="s">
+      <c r="D954" s="221" t="s">
         <v>480</v>
       </c>
-      <c r="E954" s="187"/>
-      <c r="F954" s="187"/>
-      <c r="G954" s="187"/>
-      <c r="H954" s="187"/>
-      <c r="I954" s="187"/>
-      <c r="J954" s="187"/>
-      <c r="K954" s="187"/>
+      <c r="E954" s="222"/>
+      <c r="F954" s="222"/>
+      <c r="G954" s="222"/>
+      <c r="H954" s="222"/>
+      <c r="I954" s="222"/>
+      <c r="J954" s="222"/>
+      <c r="K954" s="222"/>
     </row>
     <row r="955" spans="1:11">
       <c r="A955" s="12">
@@ -24368,32 +24476,21 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="48">
-    <mergeCell ref="D168:K168"/>
-    <mergeCell ref="D175:K175"/>
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D250:K250"/>
-    <mergeCell ref="D280:K280"/>
-    <mergeCell ref="D286:K286"/>
-    <mergeCell ref="D296:K296"/>
-    <mergeCell ref="D240:K241"/>
+  <mergeCells count="55">
+    <mergeCell ref="D95:K95"/>
+    <mergeCell ref="D96:K96"/>
+    <mergeCell ref="D90:K90"/>
+    <mergeCell ref="D91:K91"/>
+    <mergeCell ref="D92:K92"/>
+    <mergeCell ref="D93:K93"/>
+    <mergeCell ref="D94:K94"/>
+    <mergeCell ref="D954:K954"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
     <mergeCell ref="D2:K3"/>
     <mergeCell ref="D216:K217"/>
     <mergeCell ref="D218:K219"/>
@@ -24410,13 +24507,31 @@
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
     <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D954:K954"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D250:K250"/>
+    <mergeCell ref="D280:K280"/>
+    <mergeCell ref="D286:K286"/>
+    <mergeCell ref="D296:K296"/>
+    <mergeCell ref="D240:K241"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D168:K168"/>
+    <mergeCell ref="D175:K175"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape" r:id="rId1"/>
@@ -24502,16 +24617,16 @@
         <f>8*A2&amp;"-"&amp;(8*A2+7)</f>
         <v>0-7</v>
       </c>
-      <c r="D2" s="188" t="s">
+      <c r="D2" s="205" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="189"/>
-      <c r="F2" s="189"/>
-      <c r="G2" s="189"/>
-      <c r="H2" s="189"/>
-      <c r="I2" s="189"/>
-      <c r="J2" s="189"/>
-      <c r="K2" s="190"/>
+      <c r="E2" s="201"/>
+      <c r="F2" s="201"/>
+      <c r="G2" s="201"/>
+      <c r="H2" s="201"/>
+      <c r="I2" s="201"/>
+      <c r="J2" s="201"/>
+      <c r="K2" s="202"/>
       <c r="M2" s="3">
         <v>16</v>
       </c>
@@ -24533,14 +24648,14 @@
         <f t="shared" ref="C3:C33" si="2">8*A3&amp;"-"&amp;(8*A3+7)</f>
         <v>8-15</v>
       </c>
-      <c r="D3" s="191"/>
-      <c r="E3" s="192"/>
-      <c r="F3" s="192"/>
-      <c r="G3" s="192"/>
-      <c r="H3" s="192"/>
-      <c r="I3" s="192"/>
-      <c r="J3" s="192"/>
-      <c r="K3" s="196"/>
+      <c r="D3" s="211"/>
+      <c r="E3" s="195"/>
+      <c r="F3" s="195"/>
+      <c r="G3" s="195"/>
+      <c r="H3" s="195"/>
+      <c r="I3" s="195"/>
+      <c r="J3" s="195"/>
+      <c r="K3" s="208"/>
       <c r="M3" s="3">
         <v>17</v>
       </c>
@@ -30789,16 +30904,16 @@
         <v>AB0</v>
       </c>
       <c r="C178" s="38"/>
-      <c r="D178" s="221" t="s">
+      <c r="D178" s="186" t="s">
         <v>350</v>
       </c>
-      <c r="E178" s="221"/>
-      <c r="F178" s="221"/>
-      <c r="G178" s="221"/>
-      <c r="H178" s="221"/>
-      <c r="I178" s="221"/>
-      <c r="J178" s="221"/>
-      <c r="K178" s="221"/>
+      <c r="E178" s="186"/>
+      <c r="F178" s="186"/>
+      <c r="G178" s="186"/>
+      <c r="H178" s="186"/>
+      <c r="I178" s="186"/>
+      <c r="J178" s="186"/>
+      <c r="K178" s="186"/>
     </row>
     <row r="179" spans="1:14">
       <c r="A179" s="12">
@@ -30867,16 +30982,16 @@
         <v>AB4</v>
       </c>
       <c r="C182" s="13"/>
-      <c r="D182" s="204" t="s">
+      <c r="D182" s="188" t="s">
         <v>351</v>
       </c>
-      <c r="E182" s="205"/>
-      <c r="F182" s="205"/>
-      <c r="G182" s="205"/>
-      <c r="H182" s="205"/>
-      <c r="I182" s="205"/>
-      <c r="J182" s="205"/>
-      <c r="K182" s="206"/>
+      <c r="E182" s="189"/>
+      <c r="F182" s="189"/>
+      <c r="G182" s="189"/>
+      <c r="H182" s="189"/>
+      <c r="I182" s="189"/>
+      <c r="J182" s="189"/>
+      <c r="K182" s="190"/>
     </row>
     <row r="183" spans="1:14">
       <c r="A183" s="12">
@@ -30888,16 +31003,16 @@
         <v>AB5</v>
       </c>
       <c r="C183" s="13"/>
-      <c r="D183" s="204" t="s">
+      <c r="D183" s="188" t="s">
         <v>352</v>
       </c>
-      <c r="E183" s="205"/>
-      <c r="F183" s="205"/>
-      <c r="G183" s="205"/>
-      <c r="H183" s="205"/>
-      <c r="I183" s="205"/>
-      <c r="J183" s="205"/>
-      <c r="K183" s="206"/>
+      <c r="E183" s="189"/>
+      <c r="F183" s="189"/>
+      <c r="G183" s="189"/>
+      <c r="H183" s="189"/>
+      <c r="I183" s="189"/>
+      <c r="J183" s="189"/>
+      <c r="K183" s="190"/>
     </row>
     <row r="184" spans="1:14">
       <c r="A184" s="12">
@@ -30909,16 +31024,16 @@
         <v>AB6</v>
       </c>
       <c r="C184" s="13"/>
-      <c r="D184" s="204" t="s">
+      <c r="D184" s="188" t="s">
         <v>353</v>
       </c>
-      <c r="E184" s="205"/>
-      <c r="F184" s="205"/>
-      <c r="G184" s="205"/>
-      <c r="H184" s="205"/>
-      <c r="I184" s="205"/>
-      <c r="J184" s="205"/>
-      <c r="K184" s="206"/>
+      <c r="E184" s="189"/>
+      <c r="F184" s="189"/>
+      <c r="G184" s="189"/>
+      <c r="H184" s="189"/>
+      <c r="I184" s="189"/>
+      <c r="J184" s="189"/>
+      <c r="K184" s="190"/>
     </row>
     <row r="185" spans="1:14">
       <c r="A185" s="12">
@@ -30930,16 +31045,16 @@
         <v>AB7</v>
       </c>
       <c r="C185" s="13"/>
-      <c r="D185" s="204" t="s">
+      <c r="D185" s="188" t="s">
         <v>354</v>
       </c>
-      <c r="E185" s="205"/>
-      <c r="F185" s="205"/>
-      <c r="G185" s="205"/>
-      <c r="H185" s="205"/>
-      <c r="I185" s="205"/>
-      <c r="J185" s="205"/>
-      <c r="K185" s="206"/>
+      <c r="E185" s="189"/>
+      <c r="F185" s="189"/>
+      <c r="G185" s="189"/>
+      <c r="H185" s="189"/>
+      <c r="I185" s="189"/>
+      <c r="J185" s="189"/>
+      <c r="K185" s="190"/>
     </row>
     <row r="186" spans="1:14">
       <c r="A186" s="12">
@@ -30951,16 +31066,16 @@
         <v>AB8</v>
       </c>
       <c r="C186" s="13"/>
-      <c r="D186" s="204" t="s">
+      <c r="D186" s="188" t="s">
         <v>355</v>
       </c>
-      <c r="E186" s="205"/>
-      <c r="F186" s="205"/>
-      <c r="G186" s="205"/>
-      <c r="H186" s="205"/>
-      <c r="I186" s="205"/>
-      <c r="J186" s="205"/>
-      <c r="K186" s="206"/>
+      <c r="E186" s="189"/>
+      <c r="F186" s="189"/>
+      <c r="G186" s="189"/>
+      <c r="H186" s="189"/>
+      <c r="I186" s="189"/>
+      <c r="J186" s="189"/>
+      <c r="K186" s="190"/>
     </row>
     <row r="187" spans="1:14">
       <c r="A187" s="12">
@@ -30972,16 +31087,16 @@
         <v>AB9</v>
       </c>
       <c r="C187" s="13"/>
-      <c r="D187" s="204" t="s">
+      <c r="D187" s="188" t="s">
         <v>356</v>
       </c>
-      <c r="E187" s="205"/>
-      <c r="F187" s="205"/>
-      <c r="G187" s="205"/>
-      <c r="H187" s="205"/>
-      <c r="I187" s="205"/>
-      <c r="J187" s="205"/>
-      <c r="K187" s="206"/>
+      <c r="E187" s="189"/>
+      <c r="F187" s="189"/>
+      <c r="G187" s="189"/>
+      <c r="H187" s="189"/>
+      <c r="I187" s="189"/>
+      <c r="J187" s="189"/>
+      <c r="K187" s="190"/>
     </row>
     <row r="188" spans="1:14">
       <c r="A188" s="12">
@@ -30993,16 +31108,16 @@
         <v>ABA</v>
       </c>
       <c r="C188" s="13"/>
-      <c r="D188" s="204" t="s">
+      <c r="D188" s="188" t="s">
         <v>357</v>
       </c>
-      <c r="E188" s="205"/>
-      <c r="F188" s="205"/>
-      <c r="G188" s="205"/>
-      <c r="H188" s="205"/>
-      <c r="I188" s="205"/>
-      <c r="J188" s="205"/>
-      <c r="K188" s="206"/>
+      <c r="E188" s="189"/>
+      <c r="F188" s="189"/>
+      <c r="G188" s="189"/>
+      <c r="H188" s="189"/>
+      <c r="I188" s="189"/>
+      <c r="J188" s="189"/>
+      <c r="K188" s="190"/>
     </row>
     <row r="189" spans="1:14">
       <c r="A189" s="12">
@@ -31014,16 +31129,16 @@
         <v>ABB</v>
       </c>
       <c r="C189" s="13"/>
-      <c r="D189" s="204" t="s">
+      <c r="D189" s="188" t="s">
         <v>358</v>
       </c>
-      <c r="E189" s="205"/>
-      <c r="F189" s="205"/>
-      <c r="G189" s="205"/>
-      <c r="H189" s="205"/>
-      <c r="I189" s="205"/>
-      <c r="J189" s="205"/>
-      <c r="K189" s="206"/>
+      <c r="E189" s="189"/>
+      <c r="F189" s="189"/>
+      <c r="G189" s="189"/>
+      <c r="H189" s="189"/>
+      <c r="I189" s="189"/>
+      <c r="J189" s="189"/>
+      <c r="K189" s="190"/>
     </row>
     <row r="190" spans="1:14">
       <c r="A190" s="12">
@@ -31035,16 +31150,16 @@
         <v>ABC</v>
       </c>
       <c r="C190" s="13"/>
-      <c r="D190" s="204" t="s">
+      <c r="D190" s="188" t="s">
         <v>359</v>
       </c>
-      <c r="E190" s="205"/>
-      <c r="F190" s="205"/>
-      <c r="G190" s="205"/>
-      <c r="H190" s="205"/>
-      <c r="I190" s="205"/>
-      <c r="J190" s="205"/>
-      <c r="K190" s="206"/>
+      <c r="E190" s="189"/>
+      <c r="F190" s="189"/>
+      <c r="G190" s="189"/>
+      <c r="H190" s="189"/>
+      <c r="I190" s="189"/>
+      <c r="J190" s="189"/>
+      <c r="K190" s="190"/>
     </row>
     <row r="191" spans="1:14">
       <c r="A191" s="12">
@@ -31056,16 +31171,16 @@
         <v>ABD</v>
       </c>
       <c r="C191" s="13"/>
-      <c r="D191" s="204" t="s">
+      <c r="D191" s="188" t="s">
         <v>360</v>
       </c>
-      <c r="E191" s="205"/>
-      <c r="F191" s="205"/>
-      <c r="G191" s="205"/>
-      <c r="H191" s="205"/>
-      <c r="I191" s="205"/>
-      <c r="J191" s="205"/>
-      <c r="K191" s="206"/>
+      <c r="E191" s="189"/>
+      <c r="F191" s="189"/>
+      <c r="G191" s="189"/>
+      <c r="H191" s="189"/>
+      <c r="I191" s="189"/>
+      <c r="J191" s="189"/>
+      <c r="K191" s="190"/>
     </row>
     <row r="192" spans="1:14">
       <c r="A192" s="12">
@@ -31077,16 +31192,16 @@
         <v>ABE</v>
       </c>
       <c r="C192" s="13"/>
-      <c r="D192" s="204" t="s">
+      <c r="D192" s="188" t="s">
         <v>361</v>
       </c>
-      <c r="E192" s="205"/>
-      <c r="F192" s="205"/>
-      <c r="G192" s="205"/>
-      <c r="H192" s="205"/>
-      <c r="I192" s="205"/>
-      <c r="J192" s="205"/>
-      <c r="K192" s="206"/>
+      <c r="E192" s="189"/>
+      <c r="F192" s="189"/>
+      <c r="G192" s="189"/>
+      <c r="H192" s="189"/>
+      <c r="I192" s="189"/>
+      <c r="J192" s="189"/>
+      <c r="K192" s="190"/>
     </row>
     <row r="193" spans="1:14" s="1" customFormat="1">
       <c r="A193" s="31">
@@ -31098,16 +31213,16 @@
         <v>ABF</v>
       </c>
       <c r="C193" s="32"/>
-      <c r="D193" s="218" t="s">
+      <c r="D193" s="191" t="s">
         <v>362</v>
       </c>
-      <c r="E193" s="219"/>
-      <c r="F193" s="219"/>
-      <c r="G193" s="219"/>
-      <c r="H193" s="219"/>
-      <c r="I193" s="219"/>
-      <c r="J193" s="219"/>
-      <c r="K193" s="220"/>
+      <c r="E193" s="192"/>
+      <c r="F193" s="192"/>
+      <c r="G193" s="192"/>
+      <c r="H193" s="192"/>
+      <c r="I193" s="192"/>
+      <c r="J193" s="192"/>
+      <c r="K193" s="193"/>
       <c r="L193" s="56"/>
       <c r="M193" s="57"/>
       <c r="N193" s="57"/>
@@ -31122,16 +31237,16 @@
         <v>AC0</v>
       </c>
       <c r="C194" s="38"/>
-      <c r="D194" s="199" t="s">
+      <c r="D194" s="194" t="s">
         <v>363</v>
       </c>
-      <c r="E194" s="192"/>
-      <c r="F194" s="192"/>
-      <c r="G194" s="192"/>
-      <c r="H194" s="192"/>
-      <c r="I194" s="192"/>
-      <c r="J194" s="192"/>
-      <c r="K194" s="200"/>
+      <c r="E194" s="195"/>
+      <c r="F194" s="195"/>
+      <c r="G194" s="195"/>
+      <c r="H194" s="195"/>
+      <c r="I194" s="195"/>
+      <c r="J194" s="195"/>
+      <c r="K194" s="196"/>
     </row>
     <row r="195" spans="1:14">
       <c r="A195" s="12">
@@ -31143,16 +31258,16 @@
         <v>AC1</v>
       </c>
       <c r="C195" s="13"/>
-      <c r="D195" s="204" t="s">
+      <c r="D195" s="188" t="s">
         <v>364</v>
       </c>
-      <c r="E195" s="205"/>
-      <c r="F195" s="205"/>
-      <c r="G195" s="205"/>
-      <c r="H195" s="205"/>
-      <c r="I195" s="205"/>
-      <c r="J195" s="205"/>
-      <c r="K195" s="206"/>
+      <c r="E195" s="189"/>
+      <c r="F195" s="189"/>
+      <c r="G195" s="189"/>
+      <c r="H195" s="189"/>
+      <c r="I195" s="189"/>
+      <c r="J195" s="189"/>
+      <c r="K195" s="190"/>
     </row>
     <row r="196" spans="1:14">
       <c r="A196" s="12">
@@ -31164,16 +31279,16 @@
         <v>AC2</v>
       </c>
       <c r="C196" s="13"/>
-      <c r="D196" s="204" t="s">
+      <c r="D196" s="188" t="s">
         <v>365</v>
       </c>
-      <c r="E196" s="205"/>
-      <c r="F196" s="205"/>
-      <c r="G196" s="205"/>
-      <c r="H196" s="205"/>
-      <c r="I196" s="205"/>
-      <c r="J196" s="205"/>
-      <c r="K196" s="206"/>
+      <c r="E196" s="189"/>
+      <c r="F196" s="189"/>
+      <c r="G196" s="189"/>
+      <c r="H196" s="189"/>
+      <c r="I196" s="189"/>
+      <c r="J196" s="189"/>
+      <c r="K196" s="190"/>
     </row>
     <row r="197" spans="1:14">
       <c r="A197" s="12">
@@ -31185,16 +31300,16 @@
         <v>AC3</v>
       </c>
       <c r="C197" s="13"/>
-      <c r="D197" s="204" t="s">
+      <c r="D197" s="188" t="s">
         <v>366</v>
       </c>
-      <c r="E197" s="205"/>
-      <c r="F197" s="205"/>
-      <c r="G197" s="205"/>
-      <c r="H197" s="205"/>
-      <c r="I197" s="205"/>
-      <c r="J197" s="205"/>
-      <c r="K197" s="206"/>
+      <c r="E197" s="189"/>
+      <c r="F197" s="189"/>
+      <c r="G197" s="189"/>
+      <c r="H197" s="189"/>
+      <c r="I197" s="189"/>
+      <c r="J197" s="189"/>
+      <c r="K197" s="190"/>
     </row>
     <row r="198" spans="1:14">
       <c r="A198" s="12">
@@ -31206,16 +31321,16 @@
         <v>AC4</v>
       </c>
       <c r="C198" s="13"/>
-      <c r="D198" s="204" t="s">
+      <c r="D198" s="188" t="s">
         <v>367</v>
       </c>
-      <c r="E198" s="205"/>
-      <c r="F198" s="205"/>
-      <c r="G198" s="205"/>
-      <c r="H198" s="205"/>
-      <c r="I198" s="205"/>
-      <c r="J198" s="205"/>
-      <c r="K198" s="206"/>
+      <c r="E198" s="189"/>
+      <c r="F198" s="189"/>
+      <c r="G198" s="189"/>
+      <c r="H198" s="189"/>
+      <c r="I198" s="189"/>
+      <c r="J198" s="189"/>
+      <c r="K198" s="190"/>
     </row>
     <row r="199" spans="1:14">
       <c r="A199" s="12">
@@ -31246,16 +31361,16 @@
         <v>AC6</v>
       </c>
       <c r="C200" s="13"/>
-      <c r="D200" s="204" t="s">
+      <c r="D200" s="188" t="s">
         <v>368</v>
       </c>
-      <c r="E200" s="205"/>
-      <c r="F200" s="205"/>
-      <c r="G200" s="205"/>
-      <c r="H200" s="205"/>
-      <c r="I200" s="205"/>
-      <c r="J200" s="205"/>
-      <c r="K200" s="206"/>
+      <c r="E200" s="189"/>
+      <c r="F200" s="189"/>
+      <c r="G200" s="189"/>
+      <c r="H200" s="189"/>
+      <c r="I200" s="189"/>
+      <c r="J200" s="189"/>
+      <c r="K200" s="190"/>
     </row>
     <row r="201" spans="1:14">
       <c r="A201" s="12">
@@ -31286,16 +31401,16 @@
         <v>AC8</v>
       </c>
       <c r="C202" s="13"/>
-      <c r="D202" s="210" t="s">
+      <c r="D202" s="218" t="s">
         <v>369</v>
       </c>
-      <c r="E202" s="211"/>
-      <c r="F202" s="211"/>
-      <c r="G202" s="211"/>
-      <c r="H202" s="211"/>
-      <c r="I202" s="211"/>
-      <c r="J202" s="211"/>
-      <c r="K202" s="212"/>
+      <c r="E202" s="219"/>
+      <c r="F202" s="219"/>
+      <c r="G202" s="219"/>
+      <c r="H202" s="219"/>
+      <c r="I202" s="219"/>
+      <c r="J202" s="219"/>
+      <c r="K202" s="220"/>
     </row>
     <row r="203" spans="1:14">
       <c r="A203" s="12">
@@ -31326,16 +31441,16 @@
         <v>ACA</v>
       </c>
       <c r="C204" s="13"/>
-      <c r="D204" s="204" t="s">
+      <c r="D204" s="188" t="s">
         <v>370</v>
       </c>
-      <c r="E204" s="205"/>
-      <c r="F204" s="205"/>
-      <c r="G204" s="205"/>
-      <c r="H204" s="205"/>
-      <c r="I204" s="205"/>
-      <c r="J204" s="205"/>
-      <c r="K204" s="206"/>
+      <c r="E204" s="189"/>
+      <c r="F204" s="189"/>
+      <c r="G204" s="189"/>
+      <c r="H204" s="189"/>
+      <c r="I204" s="189"/>
+      <c r="J204" s="189"/>
+      <c r="K204" s="190"/>
     </row>
     <row r="205" spans="1:14">
       <c r="A205" s="12">
@@ -31366,16 +31481,16 @@
         <v>ACC</v>
       </c>
       <c r="C206" s="13"/>
-      <c r="D206" s="204" t="s">
+      <c r="D206" s="188" t="s">
         <v>370</v>
       </c>
-      <c r="E206" s="205"/>
-      <c r="F206" s="205"/>
-      <c r="G206" s="205"/>
-      <c r="H206" s="205"/>
-      <c r="I206" s="205"/>
-      <c r="J206" s="205"/>
-      <c r="K206" s="206"/>
+      <c r="E206" s="189"/>
+      <c r="F206" s="189"/>
+      <c r="G206" s="189"/>
+      <c r="H206" s="189"/>
+      <c r="I206" s="189"/>
+      <c r="J206" s="189"/>
+      <c r="K206" s="190"/>
     </row>
     <row r="207" spans="1:14">
       <c r="A207" s="12">
@@ -31406,16 +31521,16 @@
         <v>ACE</v>
       </c>
       <c r="C208" s="13"/>
-      <c r="D208" s="204" t="s">
+      <c r="D208" s="188" t="s">
         <v>371</v>
       </c>
-      <c r="E208" s="205"/>
-      <c r="F208" s="205"/>
-      <c r="G208" s="205"/>
-      <c r="H208" s="205"/>
-      <c r="I208" s="205"/>
-      <c r="J208" s="205"/>
-      <c r="K208" s="206"/>
+      <c r="E208" s="189"/>
+      <c r="F208" s="189"/>
+      <c r="G208" s="189"/>
+      <c r="H208" s="189"/>
+      <c r="I208" s="189"/>
+      <c r="J208" s="189"/>
+      <c r="K208" s="190"/>
     </row>
     <row r="209" spans="1:14" s="1" customFormat="1">
       <c r="A209" s="31">
@@ -31449,16 +31564,16 @@
         <v>AD0</v>
       </c>
       <c r="C210" s="38"/>
-      <c r="D210" s="199" t="s">
+      <c r="D210" s="194" t="s">
         <v>371</v>
       </c>
-      <c r="E210" s="192"/>
-      <c r="F210" s="192"/>
-      <c r="G210" s="192"/>
-      <c r="H210" s="192"/>
-      <c r="I210" s="192"/>
-      <c r="J210" s="192"/>
-      <c r="K210" s="200"/>
+      <c r="E210" s="195"/>
+      <c r="F210" s="195"/>
+      <c r="G210" s="195"/>
+      <c r="H210" s="195"/>
+      <c r="I210" s="195"/>
+      <c r="J210" s="195"/>
+      <c r="K210" s="196"/>
     </row>
     <row r="211" spans="1:14">
       <c r="A211" s="12">
@@ -31527,16 +31642,16 @@
         <v>AD4</v>
       </c>
       <c r="C214" s="13"/>
-      <c r="D214" s="204" t="s">
+      <c r="D214" s="188" t="s">
         <v>372</v>
       </c>
-      <c r="E214" s="205"/>
-      <c r="F214" s="205"/>
-      <c r="G214" s="205"/>
-      <c r="H214" s="205"/>
-      <c r="I214" s="205"/>
-      <c r="J214" s="205"/>
-      <c r="K214" s="206"/>
+      <c r="E214" s="189"/>
+      <c r="F214" s="189"/>
+      <c r="G214" s="189"/>
+      <c r="H214" s="189"/>
+      <c r="I214" s="189"/>
+      <c r="J214" s="189"/>
+      <c r="K214" s="190"/>
     </row>
     <row r="215" spans="1:14">
       <c r="A215" s="12">
@@ -31567,16 +31682,16 @@
         <v>AD6</v>
       </c>
       <c r="C216" s="13"/>
-      <c r="D216" s="197" t="s">
+      <c r="D216" s="209" t="s">
         <v>373</v>
       </c>
-      <c r="E216" s="189"/>
-      <c r="F216" s="189"/>
-      <c r="G216" s="189"/>
-      <c r="H216" s="189"/>
-      <c r="I216" s="189"/>
-      <c r="J216" s="189"/>
-      <c r="K216" s="198"/>
+      <c r="E216" s="201"/>
+      <c r="F216" s="201"/>
+      <c r="G216" s="201"/>
+      <c r="H216" s="201"/>
+      <c r="I216" s="201"/>
+      <c r="J216" s="201"/>
+      <c r="K216" s="210"/>
     </row>
     <row r="217" spans="1:14">
       <c r="A217" s="12">
@@ -31588,14 +31703,14 @@
         <v>AD7</v>
       </c>
       <c r="C217" s="13"/>
-      <c r="D217" s="199"/>
-      <c r="E217" s="192"/>
-      <c r="F217" s="192"/>
-      <c r="G217" s="192"/>
-      <c r="H217" s="192"/>
-      <c r="I217" s="192"/>
-      <c r="J217" s="192"/>
-      <c r="K217" s="200"/>
+      <c r="D217" s="194"/>
+      <c r="E217" s="195"/>
+      <c r="F217" s="195"/>
+      <c r="G217" s="195"/>
+      <c r="H217" s="195"/>
+      <c r="I217" s="195"/>
+      <c r="J217" s="195"/>
+      <c r="K217" s="196"/>
     </row>
     <row r="218" spans="1:14">
       <c r="A218" s="12">
@@ -31607,16 +31722,16 @@
         <v>AD8</v>
       </c>
       <c r="C218" s="13"/>
-      <c r="D218" s="197" t="s">
+      <c r="D218" s="209" t="s">
         <v>374</v>
       </c>
-      <c r="E218" s="189"/>
-      <c r="F218" s="189"/>
-      <c r="G218" s="189"/>
-      <c r="H218" s="189"/>
-      <c r="I218" s="189"/>
-      <c r="J218" s="189"/>
-      <c r="K218" s="198"/>
+      <c r="E218" s="201"/>
+      <c r="F218" s="201"/>
+      <c r="G218" s="201"/>
+      <c r="H218" s="201"/>
+      <c r="I218" s="201"/>
+      <c r="J218" s="201"/>
+      <c r="K218" s="210"/>
     </row>
     <row r="219" spans="1:14">
       <c r="A219" s="12">
@@ -31628,14 +31743,14 @@
         <v>AD9</v>
       </c>
       <c r="C219" s="13"/>
-      <c r="D219" s="199"/>
-      <c r="E219" s="192"/>
-      <c r="F219" s="192"/>
-      <c r="G219" s="192"/>
-      <c r="H219" s="192"/>
-      <c r="I219" s="192"/>
-      <c r="J219" s="192"/>
-      <c r="K219" s="200"/>
+      <c r="D219" s="194"/>
+      <c r="E219" s="195"/>
+      <c r="F219" s="195"/>
+      <c r="G219" s="195"/>
+      <c r="H219" s="195"/>
+      <c r="I219" s="195"/>
+      <c r="J219" s="195"/>
+      <c r="K219" s="196"/>
     </row>
     <row r="220" spans="1:14">
       <c r="A220" s="12">
@@ -31647,16 +31762,16 @@
         <v>ADA</v>
       </c>
       <c r="C220" s="13"/>
-      <c r="D220" s="197" t="s">
+      <c r="D220" s="209" t="s">
         <v>375</v>
       </c>
-      <c r="E220" s="189"/>
-      <c r="F220" s="189"/>
-      <c r="G220" s="189"/>
-      <c r="H220" s="189"/>
-      <c r="I220" s="189"/>
-      <c r="J220" s="189"/>
-      <c r="K220" s="198"/>
+      <c r="E220" s="201"/>
+      <c r="F220" s="201"/>
+      <c r="G220" s="201"/>
+      <c r="H220" s="201"/>
+      <c r="I220" s="201"/>
+      <c r="J220" s="201"/>
+      <c r="K220" s="210"/>
     </row>
     <row r="221" spans="1:14">
       <c r="A221" s="12">
@@ -31668,14 +31783,14 @@
         <v>ADB</v>
       </c>
       <c r="C221" s="13"/>
-      <c r="D221" s="199"/>
-      <c r="E221" s="192"/>
-      <c r="F221" s="192"/>
-      <c r="G221" s="192"/>
-      <c r="H221" s="192"/>
-      <c r="I221" s="192"/>
-      <c r="J221" s="192"/>
-      <c r="K221" s="200"/>
+      <c r="D221" s="194"/>
+      <c r="E221" s="195"/>
+      <c r="F221" s="195"/>
+      <c r="G221" s="195"/>
+      <c r="H221" s="195"/>
+      <c r="I221" s="195"/>
+      <c r="J221" s="195"/>
+      <c r="K221" s="196"/>
     </row>
     <row r="222" spans="1:14">
       <c r="A222" s="12">
@@ -31687,16 +31802,16 @@
         <v>ADC</v>
       </c>
       <c r="C222" s="13"/>
-      <c r="D222" s="204" t="s">
+      <c r="D222" s="188" t="s">
         <v>376</v>
       </c>
-      <c r="E222" s="205"/>
-      <c r="F222" s="205"/>
-      <c r="G222" s="205"/>
-      <c r="H222" s="205"/>
-      <c r="I222" s="205"/>
-      <c r="J222" s="205"/>
-      <c r="K222" s="206"/>
+      <c r="E222" s="189"/>
+      <c r="F222" s="189"/>
+      <c r="G222" s="189"/>
+      <c r="H222" s="189"/>
+      <c r="I222" s="189"/>
+      <c r="J222" s="189"/>
+      <c r="K222" s="190"/>
     </row>
     <row r="223" spans="1:14">
       <c r="A223" s="12">
@@ -31727,16 +31842,16 @@
         <v>ADE</v>
       </c>
       <c r="C224" s="13"/>
-      <c r="D224" s="204" t="s">
+      <c r="D224" s="188" t="s">
         <v>377</v>
       </c>
-      <c r="E224" s="205"/>
-      <c r="F224" s="205"/>
-      <c r="G224" s="205"/>
-      <c r="H224" s="205"/>
-      <c r="I224" s="205"/>
-      <c r="J224" s="205"/>
-      <c r="K224" s="206"/>
+      <c r="E224" s="189"/>
+      <c r="F224" s="189"/>
+      <c r="G224" s="189"/>
+      <c r="H224" s="189"/>
+      <c r="I224" s="189"/>
+      <c r="J224" s="189"/>
+      <c r="K224" s="190"/>
     </row>
     <row r="225" spans="1:14" s="1" customFormat="1">
       <c r="A225" s="31">
@@ -31770,16 +31885,16 @@
         <v>AE0</v>
       </c>
       <c r="C226" s="38"/>
-      <c r="D226" s="207" t="s">
+      <c r="D226" s="215" t="s">
         <v>378</v>
       </c>
-      <c r="E226" s="208"/>
-      <c r="F226" s="208"/>
-      <c r="G226" s="208"/>
-      <c r="H226" s="208"/>
-      <c r="I226" s="208"/>
-      <c r="J226" s="208"/>
-      <c r="K226" s="209"/>
+      <c r="E226" s="216"/>
+      <c r="F226" s="216"/>
+      <c r="G226" s="216"/>
+      <c r="H226" s="216"/>
+      <c r="I226" s="216"/>
+      <c r="J226" s="216"/>
+      <c r="K226" s="217"/>
     </row>
     <row r="227" spans="1:14">
       <c r="A227" s="12">
@@ -31924,16 +32039,16 @@
         <v>AE8</v>
       </c>
       <c r="C234" s="13"/>
-      <c r="D234" s="201" t="s">
+      <c r="D234" s="213" t="s">
         <v>379</v>
       </c>
-      <c r="E234" s="202"/>
-      <c r="F234" s="202"/>
-      <c r="G234" s="202"/>
-      <c r="H234" s="202"/>
-      <c r="I234" s="202"/>
-      <c r="J234" s="202"/>
-      <c r="K234" s="203"/>
+      <c r="E234" s="198"/>
+      <c r="F234" s="198"/>
+      <c r="G234" s="198"/>
+      <c r="H234" s="198"/>
+      <c r="I234" s="198"/>
+      <c r="J234" s="198"/>
+      <c r="K234" s="214"/>
     </row>
     <row r="235" spans="1:14">
       <c r="A235" s="12">
@@ -32002,16 +32117,16 @@
         <v>AEC</v>
       </c>
       <c r="C238" s="13"/>
-      <c r="D238" s="188" t="s">
+      <c r="D238" s="205" t="s">
         <v>380</v>
       </c>
-      <c r="E238" s="189"/>
-      <c r="F238" s="189"/>
-      <c r="G238" s="189"/>
-      <c r="H238" s="189"/>
-      <c r="I238" s="189"/>
-      <c r="J238" s="189"/>
-      <c r="K238" s="190"/>
+      <c r="E238" s="201"/>
+      <c r="F238" s="201"/>
+      <c r="G238" s="201"/>
+      <c r="H238" s="201"/>
+      <c r="I238" s="201"/>
+      <c r="J238" s="201"/>
+      <c r="K238" s="202"/>
     </row>
     <row r="239" spans="1:14">
       <c r="A239" s="12">
@@ -32023,14 +32138,14 @@
         <v>AED</v>
       </c>
       <c r="C239" s="13"/>
-      <c r="D239" s="191"/>
-      <c r="E239" s="192"/>
-      <c r="F239" s="192"/>
-      <c r="G239" s="192"/>
-      <c r="H239" s="192"/>
-      <c r="I239" s="192"/>
-      <c r="J239" s="192"/>
-      <c r="K239" s="193"/>
+      <c r="D239" s="211"/>
+      <c r="E239" s="195"/>
+      <c r="F239" s="195"/>
+      <c r="G239" s="195"/>
+      <c r="H239" s="195"/>
+      <c r="I239" s="195"/>
+      <c r="J239" s="195"/>
+      <c r="K239" s="212"/>
     </row>
     <row r="240" spans="1:14">
       <c r="A240" s="12">
@@ -32042,16 +32157,16 @@
         <v>AEE</v>
       </c>
       <c r="C240" s="68"/>
-      <c r="D240" s="189" t="s">
+      <c r="D240" s="201" t="s">
         <v>381</v>
       </c>
-      <c r="E240" s="189"/>
-      <c r="F240" s="189"/>
-      <c r="G240" s="189"/>
-      <c r="H240" s="189"/>
-      <c r="I240" s="189"/>
-      <c r="J240" s="189"/>
-      <c r="K240" s="190"/>
+      <c r="E240" s="201"/>
+      <c r="F240" s="201"/>
+      <c r="G240" s="201"/>
+      <c r="H240" s="201"/>
+      <c r="I240" s="201"/>
+      <c r="J240" s="201"/>
+      <c r="K240" s="202"/>
     </row>
     <row r="241" spans="1:14" s="1" customFormat="1">
       <c r="A241" s="31">
@@ -32063,14 +32178,14 @@
         <v>AEF</v>
       </c>
       <c r="C241" s="33"/>
-      <c r="D241" s="216"/>
-      <c r="E241" s="216"/>
-      <c r="F241" s="216"/>
-      <c r="G241" s="216"/>
-      <c r="H241" s="216"/>
-      <c r="I241" s="216"/>
-      <c r="J241" s="216"/>
-      <c r="K241" s="217"/>
+      <c r="D241" s="203"/>
+      <c r="E241" s="203"/>
+      <c r="F241" s="203"/>
+      <c r="G241" s="203"/>
+      <c r="H241" s="203"/>
+      <c r="I241" s="203"/>
+      <c r="J241" s="203"/>
+      <c r="K241" s="204"/>
       <c r="L241" s="56"/>
       <c r="M241" s="57"/>
       <c r="N241" s="57"/>
@@ -32261,16 +32376,16 @@
         <v>AF8</v>
       </c>
       <c r="C250" s="13"/>
-      <c r="D250" s="213" t="s">
+      <c r="D250" s="197" t="s">
         <v>382</v>
       </c>
-      <c r="E250" s="202"/>
-      <c r="F250" s="202"/>
-      <c r="G250" s="202"/>
-      <c r="H250" s="202"/>
-      <c r="I250" s="202"/>
-      <c r="J250" s="202"/>
-      <c r="K250" s="214"/>
+      <c r="E250" s="198"/>
+      <c r="F250" s="198"/>
+      <c r="G250" s="198"/>
+      <c r="H250" s="198"/>
+      <c r="I250" s="198"/>
+      <c r="J250" s="198"/>
+      <c r="K250" s="199"/>
     </row>
     <row r="251" spans="1:14">
       <c r="A251" s="12">
@@ -32839,16 +32954,16 @@
         <v>B16</v>
       </c>
       <c r="C280" s="13"/>
-      <c r="D280" s="204" t="s">
+      <c r="D280" s="188" t="s">
         <v>383</v>
       </c>
-      <c r="E280" s="205"/>
-      <c r="F280" s="205"/>
-      <c r="G280" s="205"/>
-      <c r="H280" s="205"/>
-      <c r="I280" s="205"/>
-      <c r="J280" s="205"/>
-      <c r="K280" s="206"/>
+      <c r="E280" s="189"/>
+      <c r="F280" s="189"/>
+      <c r="G280" s="189"/>
+      <c r="H280" s="189"/>
+      <c r="I280" s="189"/>
+      <c r="J280" s="189"/>
+      <c r="K280" s="190"/>
     </row>
     <row r="281" spans="1:14">
       <c r="A281" s="12">
@@ -32955,16 +33070,16 @@
         <v>B1C</v>
       </c>
       <c r="C286" s="13"/>
-      <c r="D286" s="204" t="s">
+      <c r="D286" s="188" t="s">
         <v>384</v>
       </c>
-      <c r="E286" s="205"/>
-      <c r="F286" s="205"/>
-      <c r="G286" s="205"/>
-      <c r="H286" s="205"/>
-      <c r="I286" s="205"/>
-      <c r="J286" s="205"/>
-      <c r="K286" s="206"/>
+      <c r="E286" s="189"/>
+      <c r="F286" s="189"/>
+      <c r="G286" s="189"/>
+      <c r="H286" s="189"/>
+      <c r="I286" s="189"/>
+      <c r="J286" s="189"/>
+      <c r="K286" s="190"/>
     </row>
     <row r="287" spans="1:14">
       <c r="A287" s="12">
@@ -33152,16 +33267,16 @@
         <v>B26</v>
       </c>
       <c r="C296" s="13"/>
-      <c r="D296" s="204" t="s">
+      <c r="D296" s="188" t="s">
         <v>386</v>
       </c>
-      <c r="E296" s="205"/>
-      <c r="F296" s="205"/>
-      <c r="G296" s="205"/>
-      <c r="H296" s="205"/>
-      <c r="I296" s="205"/>
-      <c r="J296" s="205"/>
-      <c r="K296" s="206"/>
+      <c r="E296" s="189"/>
+      <c r="F296" s="189"/>
+      <c r="G296" s="189"/>
+      <c r="H296" s="189"/>
+      <c r="I296" s="189"/>
+      <c r="J296" s="189"/>
+      <c r="K296" s="190"/>
     </row>
     <row r="297" spans="1:14">
       <c r="A297" s="12">
@@ -33192,16 +33307,16 @@
         <v>B28</v>
       </c>
       <c r="C298" s="13"/>
-      <c r="D298" s="188" t="s">
+      <c r="D298" s="205" t="s">
         <v>387</v>
       </c>
-      <c r="E298" s="189"/>
-      <c r="F298" s="189"/>
-      <c r="G298" s="189"/>
-      <c r="H298" s="189"/>
-      <c r="I298" s="189"/>
-      <c r="J298" s="189"/>
-      <c r="K298" s="190"/>
+      <c r="E298" s="201"/>
+      <c r="F298" s="201"/>
+      <c r="G298" s="201"/>
+      <c r="H298" s="201"/>
+      <c r="I298" s="201"/>
+      <c r="J298" s="201"/>
+      <c r="K298" s="202"/>
     </row>
     <row r="299" spans="1:14">
       <c r="A299" s="12">
@@ -33213,14 +33328,14 @@
         <v>B29</v>
       </c>
       <c r="C299" s="13"/>
-      <c r="D299" s="191"/>
-      <c r="E299" s="192"/>
-      <c r="F299" s="192"/>
-      <c r="G299" s="192"/>
-      <c r="H299" s="192"/>
-      <c r="I299" s="192"/>
-      <c r="J299" s="192"/>
-      <c r="K299" s="193"/>
+      <c r="D299" s="211"/>
+      <c r="E299" s="195"/>
+      <c r="F299" s="195"/>
+      <c r="G299" s="195"/>
+      <c r="H299" s="195"/>
+      <c r="I299" s="195"/>
+      <c r="J299" s="195"/>
+      <c r="K299" s="212"/>
     </row>
     <row r="300" spans="1:14">
       <c r="A300" s="12">
@@ -33232,16 +33347,16 @@
         <v>B2A</v>
       </c>
       <c r="C300" s="13"/>
-      <c r="D300" s="188" t="s">
+      <c r="D300" s="205" t="s">
         <v>388</v>
       </c>
-      <c r="E300" s="189"/>
-      <c r="F300" s="189"/>
-      <c r="G300" s="189"/>
-      <c r="H300" s="189"/>
-      <c r="I300" s="189"/>
-      <c r="J300" s="189"/>
-      <c r="K300" s="190"/>
+      <c r="E300" s="201"/>
+      <c r="F300" s="201"/>
+      <c r="G300" s="201"/>
+      <c r="H300" s="201"/>
+      <c r="I300" s="201"/>
+      <c r="J300" s="201"/>
+      <c r="K300" s="202"/>
     </row>
     <row r="301" spans="1:14">
       <c r="A301" s="12">
@@ -33253,14 +33368,14 @@
         <v>B2B</v>
       </c>
       <c r="C301" s="13"/>
-      <c r="D301" s="191"/>
-      <c r="E301" s="192"/>
-      <c r="F301" s="192"/>
-      <c r="G301" s="192"/>
-      <c r="H301" s="192"/>
-      <c r="I301" s="192"/>
-      <c r="J301" s="192"/>
-      <c r="K301" s="193"/>
+      <c r="D301" s="211"/>
+      <c r="E301" s="195"/>
+      <c r="F301" s="195"/>
+      <c r="G301" s="195"/>
+      <c r="H301" s="195"/>
+      <c r="I301" s="195"/>
+      <c r="J301" s="195"/>
+      <c r="K301" s="212"/>
     </row>
     <row r="302" spans="1:14">
       <c r="A302" s="12">
@@ -33272,16 +33387,16 @@
         <v>B2C</v>
       </c>
       <c r="C302" s="13"/>
-      <c r="D302" s="188" t="s">
+      <c r="D302" s="205" t="s">
         <v>389</v>
       </c>
-      <c r="E302" s="189"/>
-      <c r="F302" s="189"/>
-      <c r="G302" s="189"/>
-      <c r="H302" s="189"/>
-      <c r="I302" s="189"/>
-      <c r="J302" s="189"/>
-      <c r="K302" s="190"/>
+      <c r="E302" s="201"/>
+      <c r="F302" s="201"/>
+      <c r="G302" s="201"/>
+      <c r="H302" s="201"/>
+      <c r="I302" s="201"/>
+      <c r="J302" s="201"/>
+      <c r="K302" s="202"/>
     </row>
     <row r="303" spans="1:14">
       <c r="A303" s="12">
@@ -33293,14 +33408,14 @@
         <v>B2D</v>
       </c>
       <c r="C303" s="13"/>
-      <c r="D303" s="191"/>
-      <c r="E303" s="192"/>
-      <c r="F303" s="192"/>
-      <c r="G303" s="192"/>
-      <c r="H303" s="192"/>
-      <c r="I303" s="192"/>
-      <c r="J303" s="192"/>
-      <c r="K303" s="193"/>
+      <c r="D303" s="211"/>
+      <c r="E303" s="195"/>
+      <c r="F303" s="195"/>
+      <c r="G303" s="195"/>
+      <c r="H303" s="195"/>
+      <c r="I303" s="195"/>
+      <c r="J303" s="195"/>
+      <c r="K303" s="212"/>
     </row>
     <row r="304" spans="1:14">
       <c r="A304" s="12">
@@ -33312,16 +33427,16 @@
         <v>B2E</v>
       </c>
       <c r="C304" s="13"/>
-      <c r="D304" s="188" t="s">
+      <c r="D304" s="205" t="s">
         <v>390</v>
       </c>
-      <c r="E304" s="189"/>
-      <c r="F304" s="189"/>
-      <c r="G304" s="189"/>
-      <c r="H304" s="189"/>
-      <c r="I304" s="189"/>
-      <c r="J304" s="189"/>
-      <c r="K304" s="190"/>
+      <c r="E304" s="201"/>
+      <c r="F304" s="201"/>
+      <c r="G304" s="201"/>
+      <c r="H304" s="201"/>
+      <c r="I304" s="201"/>
+      <c r="J304" s="201"/>
+      <c r="K304" s="202"/>
     </row>
     <row r="305" spans="1:14" s="1" customFormat="1">
       <c r="A305" s="31">
@@ -33333,14 +33448,14 @@
         <v>B2F</v>
       </c>
       <c r="C305" s="32"/>
-      <c r="D305" s="191"/>
-      <c r="E305" s="192"/>
-      <c r="F305" s="192"/>
-      <c r="G305" s="192"/>
-      <c r="H305" s="192"/>
-      <c r="I305" s="192"/>
-      <c r="J305" s="192"/>
-      <c r="K305" s="193"/>
+      <c r="D305" s="211"/>
+      <c r="E305" s="195"/>
+      <c r="F305" s="195"/>
+      <c r="G305" s="195"/>
+      <c r="H305" s="195"/>
+      <c r="I305" s="195"/>
+      <c r="J305" s="195"/>
+      <c r="K305" s="212"/>
       <c r="L305" s="56"/>
       <c r="M305" s="57"/>
       <c r="N305" s="57"/>
@@ -33355,16 +33470,16 @@
         <v>B30</v>
       </c>
       <c r="C306" s="38"/>
-      <c r="D306" s="188" t="s">
+      <c r="D306" s="205" t="s">
         <v>391</v>
       </c>
-      <c r="E306" s="189"/>
-      <c r="F306" s="189"/>
-      <c r="G306" s="189"/>
-      <c r="H306" s="189"/>
-      <c r="I306" s="189"/>
-      <c r="J306" s="189"/>
-      <c r="K306" s="190"/>
+      <c r="E306" s="201"/>
+      <c r="F306" s="201"/>
+      <c r="G306" s="201"/>
+      <c r="H306" s="201"/>
+      <c r="I306" s="201"/>
+      <c r="J306" s="201"/>
+      <c r="K306" s="202"/>
     </row>
     <row r="307" spans="1:14">
       <c r="A307" s="12">
@@ -33376,14 +33491,14 @@
         <v>B31</v>
       </c>
       <c r="C307" s="13"/>
-      <c r="D307" s="191"/>
-      <c r="E307" s="192"/>
-      <c r="F307" s="192"/>
-      <c r="G307" s="192"/>
-      <c r="H307" s="192"/>
-      <c r="I307" s="192"/>
-      <c r="J307" s="192"/>
-      <c r="K307" s="193"/>
+      <c r="D307" s="211"/>
+      <c r="E307" s="195"/>
+      <c r="F307" s="195"/>
+      <c r="G307" s="195"/>
+      <c r="H307" s="195"/>
+      <c r="I307" s="195"/>
+      <c r="J307" s="195"/>
+      <c r="K307" s="212"/>
     </row>
     <row r="308" spans="1:14">
       <c r="A308" s="12">
@@ -33395,16 +33510,16 @@
         <v>B32</v>
       </c>
       <c r="C308" s="13"/>
-      <c r="D308" s="188" t="s">
+      <c r="D308" s="205" t="s">
         <v>392</v>
       </c>
-      <c r="E308" s="189"/>
-      <c r="F308" s="189"/>
-      <c r="G308" s="189"/>
-      <c r="H308" s="189"/>
-      <c r="I308" s="189"/>
-      <c r="J308" s="189"/>
-      <c r="K308" s="190"/>
+      <c r="E308" s="201"/>
+      <c r="F308" s="201"/>
+      <c r="G308" s="201"/>
+      <c r="H308" s="201"/>
+      <c r="I308" s="201"/>
+      <c r="J308" s="201"/>
+      <c r="K308" s="202"/>
     </row>
     <row r="309" spans="1:14">
       <c r="A309" s="12">
@@ -33416,14 +33531,14 @@
         <v>B33</v>
       </c>
       <c r="C309" s="13"/>
-      <c r="D309" s="191"/>
-      <c r="E309" s="192"/>
-      <c r="F309" s="192"/>
-      <c r="G309" s="192"/>
-      <c r="H309" s="192"/>
-      <c r="I309" s="192"/>
-      <c r="J309" s="192"/>
-      <c r="K309" s="193"/>
+      <c r="D309" s="211"/>
+      <c r="E309" s="195"/>
+      <c r="F309" s="195"/>
+      <c r="G309" s="195"/>
+      <c r="H309" s="195"/>
+      <c r="I309" s="195"/>
+      <c r="J309" s="195"/>
+      <c r="K309" s="212"/>
     </row>
     <row r="310" spans="1:14">
       <c r="A310" s="12">
@@ -37303,29 +37418,12 @@
     </row>
   </sheetData>
   <mergeCells count="45">
-    <mergeCell ref="D178:K178"/>
-    <mergeCell ref="D182:K182"/>
-    <mergeCell ref="D183:K183"/>
-    <mergeCell ref="D184:K184"/>
-    <mergeCell ref="D185:K185"/>
-    <mergeCell ref="D186:K186"/>
-    <mergeCell ref="D187:K187"/>
-    <mergeCell ref="D188:K188"/>
-    <mergeCell ref="D189:K189"/>
-    <mergeCell ref="D190:K190"/>
-    <mergeCell ref="D191:K191"/>
-    <mergeCell ref="D192:K192"/>
-    <mergeCell ref="D193:K193"/>
-    <mergeCell ref="D194:K194"/>
-    <mergeCell ref="D195:K195"/>
-    <mergeCell ref="D208:K208"/>
-    <mergeCell ref="D210:K210"/>
-    <mergeCell ref="D214:K214"/>
-    <mergeCell ref="D196:K196"/>
-    <mergeCell ref="D197:K197"/>
-    <mergeCell ref="D198:K198"/>
-    <mergeCell ref="D200:K200"/>
-    <mergeCell ref="D202:K202"/>
+    <mergeCell ref="D308:K309"/>
+    <mergeCell ref="D298:K299"/>
+    <mergeCell ref="D300:K301"/>
+    <mergeCell ref="D302:K303"/>
+    <mergeCell ref="D304:K305"/>
+    <mergeCell ref="D306:K307"/>
     <mergeCell ref="D280:K280"/>
     <mergeCell ref="D286:K286"/>
     <mergeCell ref="D296:K296"/>
@@ -37342,12 +37440,29 @@
     <mergeCell ref="D250:K250"/>
     <mergeCell ref="D204:K204"/>
     <mergeCell ref="D206:K206"/>
-    <mergeCell ref="D308:K309"/>
-    <mergeCell ref="D298:K299"/>
-    <mergeCell ref="D300:K301"/>
-    <mergeCell ref="D302:K303"/>
-    <mergeCell ref="D304:K305"/>
-    <mergeCell ref="D306:K307"/>
+    <mergeCell ref="D208:K208"/>
+    <mergeCell ref="D210:K210"/>
+    <mergeCell ref="D214:K214"/>
+    <mergeCell ref="D196:K196"/>
+    <mergeCell ref="D197:K197"/>
+    <mergeCell ref="D198:K198"/>
+    <mergeCell ref="D200:K200"/>
+    <mergeCell ref="D202:K202"/>
+    <mergeCell ref="D191:K191"/>
+    <mergeCell ref="D192:K192"/>
+    <mergeCell ref="D193:K193"/>
+    <mergeCell ref="D194:K194"/>
+    <mergeCell ref="D195:K195"/>
+    <mergeCell ref="D186:K186"/>
+    <mergeCell ref="D187:K187"/>
+    <mergeCell ref="D188:K188"/>
+    <mergeCell ref="D189:K189"/>
+    <mergeCell ref="D190:K190"/>
+    <mergeCell ref="D178:K178"/>
+    <mergeCell ref="D182:K182"/>
+    <mergeCell ref="D183:K183"/>
+    <mergeCell ref="D184:K184"/>
+    <mergeCell ref="D185:K185"/>
   </mergeCells>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="53" fitToHeight="0" orientation="landscape"/>

</xml_diff>